<commit_message>
Fix formatting, closes #203
</commit_message>
<xml_diff>
--- a/server/assets/uctovani-v6.xlsx
+++ b/server/assets/uctovani-v6.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\micro\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\micro\Práce\bosan\bosan.cz\server\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9175FFD0-BE70-4C9A-9B4C-0A780C6162F3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46657CC9-BCF5-4A90-8801-9A8545481DE9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32760" yWindow="32760" windowWidth="16380" windowHeight="8190" tabRatio="512" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="512" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Souhrnný AKCE_TABORY" sheetId="1" state="hidden" r:id="rId1"/>
@@ -34,6 +34,13 @@
     <definedName name="_xlnm.Print_Area" localSheetId="7">'Seznam účastníků'!$A$1:$F$44</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -2420,7 +2427,7 @@
     <xf numFmtId="164" fontId="54" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="54" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="286">
+  <cellXfs count="287">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
@@ -2887,6 +2894,20 @@
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="45" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="45" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
@@ -2912,20 +2933,46 @@
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="171" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="172" fontId="22" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="170" fontId="16" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="19" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="170" fontId="16" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="170" fontId="21" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="21" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="167" fontId="21" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="1" fontId="10" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2948,52 +2995,43 @@
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="21" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="19" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="21" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
-      <protection locked="0"/>
     </xf>
-    <xf numFmtId="170" fontId="21" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="169" fontId="1" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="170" fontId="16" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="171" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="172" fontId="22" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="170" fontId="16" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="35" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="169" fontId="35" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="37" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="35" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="169" fontId="36" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="169" fontId="35" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="169" fontId="36" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -3017,26 +3055,18 @@
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="36" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="169" fontId="35" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="35" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="169" fontId="35" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="37" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -3053,16 +3083,11 @@
     <xf numFmtId="0" fontId="29" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="45" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -3080,22 +3105,8 @@
       <alignment horizontal="justify" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="45" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="45" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="45" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -5456,26 +5467,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="217" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="217"/>
-      <c r="C1" s="217"/>
-      <c r="D1" s="217"/>
-      <c r="E1" s="217"/>
-      <c r="F1" s="217"/>
-      <c r="G1" s="217"/>
+      <c r="A1" s="222" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="222"/>
+      <c r="C1" s="222"/>
+      <c r="D1" s="222"/>
+      <c r="E1" s="222"/>
+      <c r="F1" s="222"/>
+      <c r="G1" s="222"/>
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" ht="29.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="218" t="s">
+      <c r="A2" s="223" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="218"/>
-      <c r="C2" s="218"/>
-      <c r="D2" s="218"/>
-      <c r="E2" s="218"/>
-      <c r="F2" s="218"/>
-      <c r="G2" s="218"/>
+      <c r="B2" s="223"/>
+      <c r="C2" s="223"/>
+      <c r="D2" s="223"/>
+      <c r="E2" s="223"/>
+      <c r="F2" s="223"/>
+      <c r="G2" s="223"/>
     </row>
     <row r="3" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
@@ -5484,7 +5495,7 @@
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
-      <c r="G3" s="219"/>
+      <c r="G3" s="224"/>
     </row>
     <row r="4" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3"/>
@@ -5493,7 +5504,7 @@
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
-      <c r="G4" s="219"/>
+      <c r="G4" s="224"/>
     </row>
     <row r="5" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3"/>
@@ -5502,7 +5513,7 @@
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
-      <c r="G5" s="219"/>
+      <c r="G5" s="224"/>
     </row>
     <row r="6" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5"/>
@@ -5568,11 +5579,11 @@
       <c r="A12" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="220"/>
-      <c r="D12" s="220"/>
-      <c r="E12" s="220"/>
-      <c r="F12" s="220"/>
-      <c r="G12" s="220"/>
+      <c r="C12" s="225"/>
+      <c r="D12" s="225"/>
+      <c r="E12" s="225"/>
+      <c r="F12" s="225"/>
+      <c r="G12" s="225"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="15"/>
@@ -5593,10 +5604,10 @@
       <c r="D14" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="E14" s="221" t="s">
+      <c r="E14" s="226" t="s">
         <v>8</v>
       </c>
-      <c r="F14" s="221"/>
+      <c r="F14" s="226"/>
       <c r="G14" s="21" t="s">
         <v>9</v>
       </c>
@@ -5612,10 +5623,10 @@
       <c r="D15" s="23">
         <v>40195</v>
       </c>
-      <c r="E15" s="222" t="s">
+      <c r="E15" s="227" t="s">
         <v>11</v>
       </c>
-      <c r="F15" s="222"/>
+      <c r="F15" s="227"/>
       <c r="G15" s="24">
         <v>1000</v>
       </c>
@@ -5627,8 +5638,8 @@
       </c>
       <c r="C16" s="25"/>
       <c r="D16" s="25"/>
-      <c r="E16" s="216"/>
-      <c r="F16" s="216"/>
+      <c r="E16" s="221"/>
+      <c r="F16" s="221"/>
       <c r="G16" s="24"/>
     </row>
     <row r="17" spans="1:7" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.4">
@@ -5638,8 +5649,8 @@
       </c>
       <c r="C17" s="25"/>
       <c r="D17" s="25"/>
-      <c r="E17" s="216"/>
-      <c r="F17" s="216"/>
+      <c r="E17" s="221"/>
+      <c r="F17" s="221"/>
       <c r="G17" s="24"/>
     </row>
     <row r="18" spans="1:7" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.4">
@@ -5649,8 +5660,8 @@
       </c>
       <c r="C18" s="25"/>
       <c r="D18" s="25"/>
-      <c r="E18" s="216"/>
-      <c r="F18" s="216"/>
+      <c r="E18" s="221"/>
+      <c r="F18" s="221"/>
       <c r="G18" s="24"/>
     </row>
     <row r="19" spans="1:7" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.4">
@@ -5660,8 +5671,8 @@
       </c>
       <c r="C19" s="25"/>
       <c r="D19" s="25"/>
-      <c r="E19" s="216"/>
-      <c r="F19" s="216"/>
+      <c r="E19" s="221"/>
+      <c r="F19" s="221"/>
       <c r="G19" s="24"/>
     </row>
     <row r="20" spans="1:7" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -5671,8 +5682,8 @@
       </c>
       <c r="C20" s="25"/>
       <c r="D20" s="25"/>
-      <c r="E20" s="216"/>
-      <c r="F20" s="216"/>
+      <c r="E20" s="221"/>
+      <c r="F20" s="221"/>
       <c r="G20" s="24"/>
     </row>
     <row r="21" spans="1:7" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -5682,8 +5693,8 @@
       </c>
       <c r="C21" s="25"/>
       <c r="D21" s="25"/>
-      <c r="E21" s="216"/>
-      <c r="F21" s="216"/>
+      <c r="E21" s="221"/>
+      <c r="F21" s="221"/>
       <c r="G21" s="24"/>
     </row>
     <row r="22" spans="1:7" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -5693,8 +5704,8 @@
       </c>
       <c r="C22" s="25"/>
       <c r="D22" s="25"/>
-      <c r="E22" s="216"/>
-      <c r="F22" s="216"/>
+      <c r="E22" s="221"/>
+      <c r="F22" s="221"/>
       <c r="G22" s="24"/>
     </row>
     <row r="23" spans="1:7" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -5704,8 +5715,8 @@
       </c>
       <c r="C23" s="25"/>
       <c r="D23" s="25"/>
-      <c r="E23" s="216"/>
-      <c r="F23" s="216"/>
+      <c r="E23" s="221"/>
+      <c r="F23" s="221"/>
       <c r="G23" s="24"/>
     </row>
     <row r="24" spans="1:7" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -5715,8 +5726,8 @@
       </c>
       <c r="C24" s="25"/>
       <c r="D24" s="25"/>
-      <c r="E24" s="216"/>
-      <c r="F24" s="216"/>
+      <c r="E24" s="221"/>
+      <c r="F24" s="221"/>
       <c r="G24" s="24"/>
     </row>
     <row r="25" spans="1:7" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -5726,8 +5737,8 @@
       </c>
       <c r="C25" s="25"/>
       <c r="D25" s="25"/>
-      <c r="E25" s="216"/>
-      <c r="F25" s="216"/>
+      <c r="E25" s="221"/>
+      <c r="F25" s="221"/>
       <c r="G25" s="24"/>
     </row>
     <row r="26" spans="1:7" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -5737,8 +5748,8 @@
       </c>
       <c r="C26" s="25"/>
       <c r="D26" s="25"/>
-      <c r="E26" s="216"/>
-      <c r="F26" s="216"/>
+      <c r="E26" s="221"/>
+      <c r="F26" s="221"/>
       <c r="G26" s="24"/>
     </row>
     <row r="27" spans="1:7" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -5748,8 +5759,8 @@
       </c>
       <c r="C27" s="25"/>
       <c r="D27" s="25"/>
-      <c r="E27" s="216"/>
-      <c r="F27" s="216"/>
+      <c r="E27" s="221"/>
+      <c r="F27" s="221"/>
       <c r="G27" s="24"/>
     </row>
     <row r="28" spans="1:7" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -5759,8 +5770,8 @@
       </c>
       <c r="C28" s="25"/>
       <c r="D28" s="25"/>
-      <c r="E28" s="216"/>
-      <c r="F28" s="216"/>
+      <c r="E28" s="221"/>
+      <c r="F28" s="221"/>
       <c r="G28" s="24"/>
     </row>
     <row r="29" spans="1:7" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -5770,8 +5781,8 @@
       </c>
       <c r="C29" s="25"/>
       <c r="D29" s="25"/>
-      <c r="E29" s="216"/>
-      <c r="F29" s="216"/>
+      <c r="E29" s="221"/>
+      <c r="F29" s="221"/>
       <c r="G29" s="24"/>
     </row>
     <row r="30" spans="1:7" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -5781,8 +5792,8 @@
       </c>
       <c r="C30" s="25"/>
       <c r="D30" s="25"/>
-      <c r="E30" s="216"/>
-      <c r="F30" s="216"/>
+      <c r="E30" s="221"/>
+      <c r="F30" s="221"/>
       <c r="G30" s="24"/>
     </row>
     <row r="31" spans="1:7" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -5792,8 +5803,8 @@
       </c>
       <c r="C31" s="25"/>
       <c r="D31" s="25"/>
-      <c r="E31" s="216"/>
-      <c r="F31" s="216"/>
+      <c r="E31" s="221"/>
+      <c r="F31" s="221"/>
       <c r="G31" s="24"/>
     </row>
     <row r="32" spans="1:7" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -5803,8 +5814,8 @@
       </c>
       <c r="C32" s="25"/>
       <c r="D32" s="25"/>
-      <c r="E32" s="216"/>
-      <c r="F32" s="216"/>
+      <c r="E32" s="221"/>
+      <c r="F32" s="221"/>
       <c r="G32" s="24"/>
     </row>
     <row r="33" spans="1:7" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -5814,8 +5825,8 @@
       </c>
       <c r="C33" s="25"/>
       <c r="D33" s="25"/>
-      <c r="E33" s="216"/>
-      <c r="F33" s="216"/>
+      <c r="E33" s="221"/>
+      <c r="F33" s="221"/>
       <c r="G33" s="24"/>
     </row>
     <row r="34" spans="1:7" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -5825,8 +5836,8 @@
       </c>
       <c r="C34" s="25"/>
       <c r="D34" s="25"/>
-      <c r="E34" s="216"/>
-      <c r="F34" s="216"/>
+      <c r="E34" s="221"/>
+      <c r="F34" s="221"/>
       <c r="G34" s="24"/>
     </row>
     <row r="35" spans="1:7" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -5836,8 +5847,8 @@
       </c>
       <c r="C35" s="25"/>
       <c r="D35" s="25"/>
-      <c r="E35" s="216"/>
-      <c r="F35" s="216"/>
+      <c r="E35" s="221"/>
+      <c r="F35" s="221"/>
       <c r="G35" s="24"/>
     </row>
     <row r="36" spans="1:7" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -5847,8 +5858,8 @@
       </c>
       <c r="C36" s="25"/>
       <c r="D36" s="25"/>
-      <c r="E36" s="216"/>
-      <c r="F36" s="216"/>
+      <c r="E36" s="221"/>
+      <c r="F36" s="221"/>
       <c r="G36" s="24"/>
     </row>
     <row r="37" spans="1:7" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -5858,8 +5869,8 @@
       </c>
       <c r="C37" s="25"/>
       <c r="D37" s="25"/>
-      <c r="E37" s="216"/>
-      <c r="F37" s="216"/>
+      <c r="E37" s="221"/>
+      <c r="F37" s="221"/>
       <c r="G37" s="24"/>
     </row>
     <row r="38" spans="1:7" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -5869,8 +5880,8 @@
       </c>
       <c r="C38" s="25"/>
       <c r="D38" s="25"/>
-      <c r="E38" s="216"/>
-      <c r="F38" s="216"/>
+      <c r="E38" s="221"/>
+      <c r="F38" s="221"/>
       <c r="G38" s="24"/>
     </row>
     <row r="39" spans="1:7" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -5880,8 +5891,8 @@
       </c>
       <c r="C39" s="25"/>
       <c r="D39" s="25"/>
-      <c r="E39" s="216"/>
-      <c r="F39" s="216"/>
+      <c r="E39" s="221"/>
+      <c r="F39" s="221"/>
       <c r="G39" s="24"/>
     </row>
     <row r="40" spans="1:7" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -5891,8 +5902,8 @@
       </c>
       <c r="C40" s="25"/>
       <c r="D40" s="25"/>
-      <c r="E40" s="216"/>
-      <c r="F40" s="216"/>
+      <c r="E40" s="221"/>
+      <c r="F40" s="221"/>
       <c r="G40" s="24"/>
     </row>
     <row r="41" spans="1:7" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -5902,8 +5913,8 @@
       </c>
       <c r="C41" s="25"/>
       <c r="D41" s="25"/>
-      <c r="E41" s="216"/>
-      <c r="F41" s="216"/>
+      <c r="E41" s="221"/>
+      <c r="F41" s="221"/>
       <c r="G41" s="24"/>
     </row>
     <row r="42" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -5946,14 +5957,18 @@
   </sheetData>
   <sheetProtection sheet="1"/>
   <mergeCells count="32">
-    <mergeCell ref="E40:F40"/>
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="G3:G5"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="E20:F20"/>
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E22:F22"/>
     <mergeCell ref="E23:F23"/>
@@ -5966,18 +5981,14 @@
     <mergeCell ref="E30:F30"/>
     <mergeCell ref="E31:F31"/>
     <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="G3:G5"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="E39:F39"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0527777777777778" bottom="1.0527777777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -6026,54 +6037,54 @@
       <c r="A4" s="156" t="s">
         <v>193</v>
       </c>
-      <c r="B4" s="273">
+      <c r="B4" s="279">
         <f>'Seznam účastníků'!B4</f>
         <v>0</v>
       </c>
-      <c r="C4" s="273"/>
+      <c r="C4" s="279"/>
       <c r="D4"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="156" t="s">
         <v>194</v>
       </c>
-      <c r="B5" s="274">
+      <c r="B5" s="280">
         <f>'Seznam účastníků'!B5</f>
         <v>0</v>
       </c>
-      <c r="C5" s="274"/>
+      <c r="C5" s="280"/>
       <c r="D5"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="156" t="s">
         <v>195</v>
       </c>
-      <c r="B6" s="274">
+      <c r="B6" s="280">
         <f>'Seznam účastníků'!B6</f>
         <v>0</v>
       </c>
-      <c r="C6" s="274"/>
+      <c r="C6" s="280"/>
       <c r="D6"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="156" t="s">
         <v>196</v>
       </c>
-      <c r="B7" s="273">
+      <c r="B7" s="279">
         <f>'Seznam účastníků'!B7</f>
         <v>0</v>
       </c>
-      <c r="C7" s="273"/>
+      <c r="C7" s="279"/>
       <c r="D7"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="168"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="276" t="s">
+      <c r="A9" s="282" t="s">
         <v>211</v>
       </c>
-      <c r="B9" s="276"/>
+      <c r="B9" s="282"/>
     </row>
     <row r="11" spans="1:14" s="157" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="193" t="s">
@@ -6598,20 +6609,20 @@
       <c r="L45" s="35"/>
     </row>
     <row r="46" spans="1:14" s="159" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B46" s="275" t="s">
+      <c r="B46" s="281" t="s">
         <v>214</v>
       </c>
-      <c r="C46" s="275"/>
+      <c r="C46" s="281"/>
       <c r="D46" s="197" t="e">
         <f>'Soupis výdajů'!D44/'Přehled o vybraných poplatcích'!D49</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="47" spans="1:14" s="159" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B47" s="275" t="s">
+      <c r="B47" s="281" t="s">
         <v>215</v>
       </c>
-      <c r="C47" s="275"/>
+      <c r="C47" s="281"/>
       <c r="D47" s="197" t="e">
         <f>ROUND(D46/5,0)*5</f>
         <v>#DIV/0!</v>
@@ -6766,50 +6777,50 @@
       <c r="A4" s="156" t="s">
         <v>193</v>
       </c>
-      <c r="B4" s="273">
+      <c r="B4" s="279">
         <f>'Seznam účastníků'!B4</f>
         <v>0</v>
       </c>
-      <c r="C4" s="273"/>
+      <c r="C4" s="279"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="156" t="s">
         <v>194</v>
       </c>
-      <c r="B5" s="274">
+      <c r="B5" s="280">
         <f>'Seznam účastníků'!B5</f>
         <v>0</v>
       </c>
-      <c r="C5" s="274"/>
+      <c r="C5" s="280"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="156" t="s">
         <v>195</v>
       </c>
-      <c r="B6" s="274">
+      <c r="B6" s="280">
         <f>'Seznam účastníků'!B6</f>
         <v>0</v>
       </c>
-      <c r="C6" s="274"/>
+      <c r="C6" s="280"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="156" t="s">
         <v>196</v>
       </c>
-      <c r="B7" s="273">
+      <c r="B7" s="279">
         <f>'Seznam účastníků'!B7</f>
         <v>0</v>
       </c>
-      <c r="C7" s="273"/>
+      <c r="C7" s="279"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="205"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="277" t="s">
+      <c r="A9" s="283" t="s">
         <v>220</v>
       </c>
-      <c r="B9" s="277"/>
+      <c r="B9" s="283"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="206"/>
@@ -6818,12 +6829,12 @@
       <c r="A11" s="207"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="277" t="s">
+      <c r="A19" s="283" t="s">
         <v>221</v>
       </c>
-      <c r="B19" s="277"/>
-      <c r="C19" s="277"/>
-      <c r="D19" s="277"/>
+      <c r="B19" s="283"/>
+      <c r="C19" s="283"/>
+      <c r="D19" s="283"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="206" t="s">
@@ -6834,13 +6845,13 @@
       <c r="A21" s="206"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="277" t="s">
+      <c r="A22" s="283" t="s">
         <v>223</v>
       </c>
-      <c r="B22" s="277"/>
-      <c r="C22" s="277"/>
-      <c r="D22" s="277"/>
-      <c r="E22" s="277"/>
+      <c r="B22" s="283"/>
+      <c r="C22" s="283"/>
+      <c r="D22" s="283"/>
+      <c r="E22" s="283"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="206" t="s">
@@ -6851,13 +6862,13 @@
       <c r="A24" s="206"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="277" t="s">
+      <c r="A25" s="283" t="s">
         <v>224</v>
       </c>
-      <c r="B25" s="277"/>
-      <c r="C25" s="277"/>
-      <c r="D25" s="277"/>
-      <c r="E25" s="277"/>
+      <c r="B25" s="283"/>
+      <c r="C25" s="283"/>
+      <c r="D25" s="283"/>
+      <c r="E25" s="283"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="206" t="s">
@@ -6868,14 +6879,14 @@
       <c r="A27" s="206"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" s="277" t="s">
+      <c r="A28" s="283" t="s">
         <v>225</v>
       </c>
-      <c r="B28" s="277"/>
-      <c r="C28" s="277"/>
-      <c r="D28" s="277"/>
-      <c r="E28" s="277"/>
-      <c r="F28" s="277"/>
+      <c r="B28" s="283"/>
+      <c r="C28" s="283"/>
+      <c r="D28" s="283"/>
+      <c r="E28" s="283"/>
+      <c r="F28" s="283"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
@@ -6924,28 +6935,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="217" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="217"/>
-      <c r="C1" s="217"/>
-      <c r="D1" s="217"/>
-      <c r="E1" s="217"/>
-      <c r="F1" s="217"/>
-      <c r="G1" s="217"/>
+      <c r="A1" s="222" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="222"/>
+      <c r="C1" s="222"/>
+      <c r="D1" s="222"/>
+      <c r="E1" s="222"/>
+      <c r="F1" s="222"/>
+      <c r="G1" s="222"/>
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="218" t="str">
+      <c r="A2" s="223" t="str">
         <f>'Formulář  AKCE'!B2</f>
         <v>smlouvy č. DAG/61/03/001435/2009 o poskytnutí finančních prostředků
 Příloha k vyúčtování akcí a táborů</v>
       </c>
-      <c r="B2" s="218"/>
-      <c r="C2" s="218"/>
-      <c r="D2" s="218"/>
-      <c r="E2" s="218"/>
-      <c r="F2" s="218"/>
-      <c r="G2" s="218"/>
+      <c r="B2" s="223"/>
+      <c r="C2" s="223"/>
+      <c r="D2" s="223"/>
+      <c r="E2" s="223"/>
+      <c r="F2" s="223"/>
+      <c r="G2" s="223"/>
     </row>
     <row r="3" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
@@ -6954,7 +6965,7 @@
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
-      <c r="G3" s="278" t="str">
+      <c r="G3" s="284" t="str">
         <f>IF(ISNUMBER('Formulář  AKCE'!G3),'Formulář  AKCE'!G3," ")</f>
         <v xml:space="preserve"> </v>
       </c>
@@ -6966,7 +6977,7 @@
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
-      <c r="G4" s="278"/>
+      <c r="G4" s="284"/>
     </row>
     <row r="5" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3"/>
@@ -6975,7 +6986,7 @@
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
-      <c r="G5" s="278"/>
+      <c r="G5" s="284"/>
     </row>
     <row r="6" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5"/>
@@ -7025,237 +7036,237 @@
       <c r="A11" s="15">
         <v>3</v>
       </c>
-      <c r="B11" s="279" t="s">
+      <c r="B11" s="285" t="s">
         <v>227</v>
       </c>
-      <c r="C11" s="279"/>
-      <c r="D11" s="279"/>
-      <c r="E11" s="279"/>
-      <c r="F11" s="279"/>
-      <c r="G11" s="279"/>
+      <c r="C11" s="285"/>
+      <c r="D11" s="285"/>
+      <c r="E11" s="285"/>
+      <c r="F11" s="285"/>
+      <c r="G11" s="285"/>
     </row>
     <row r="12" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="29"/>
-      <c r="B12" s="279"/>
-      <c r="C12" s="279"/>
-      <c r="D12" s="279"/>
-      <c r="E12" s="279"/>
-      <c r="F12" s="279"/>
-      <c r="G12" s="279"/>
+      <c r="B12" s="285"/>
+      <c r="C12" s="285"/>
+      <c r="D12" s="285"/>
+      <c r="E12" s="285"/>
+      <c r="F12" s="285"/>
+      <c r="G12" s="285"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B13" s="279"/>
-      <c r="C13" s="279"/>
-      <c r="D13" s="279"/>
-      <c r="E13" s="279"/>
-      <c r="F13" s="279"/>
-      <c r="G13" s="279"/>
+      <c r="B13" s="285"/>
+      <c r="C13" s="285"/>
+      <c r="D13" s="285"/>
+      <c r="E13" s="285"/>
+      <c r="F13" s="285"/>
+      <c r="G13" s="285"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B14" s="279"/>
-      <c r="C14" s="279"/>
-      <c r="D14" s="279"/>
-      <c r="E14" s="279"/>
-      <c r="F14" s="279"/>
-      <c r="G14" s="279"/>
+      <c r="B14" s="285"/>
+      <c r="C14" s="285"/>
+      <c r="D14" s="285"/>
+      <c r="E14" s="285"/>
+      <c r="F14" s="285"/>
+      <c r="G14" s="285"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B15" s="279"/>
-      <c r="C15" s="279"/>
-      <c r="D15" s="279"/>
-      <c r="E15" s="279"/>
-      <c r="F15" s="279"/>
-      <c r="G15" s="279"/>
+      <c r="B15" s="285"/>
+      <c r="C15" s="285"/>
+      <c r="D15" s="285"/>
+      <c r="E15" s="285"/>
+      <c r="F15" s="285"/>
+      <c r="G15" s="285"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B16" s="279"/>
-      <c r="C16" s="279"/>
-      <c r="D16" s="279"/>
-      <c r="E16" s="279"/>
-      <c r="F16" s="279"/>
-      <c r="G16" s="279"/>
+      <c r="B16" s="285"/>
+      <c r="C16" s="285"/>
+      <c r="D16" s="285"/>
+      <c r="E16" s="285"/>
+      <c r="F16" s="285"/>
+      <c r="G16" s="285"/>
     </row>
     <row r="17" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="279"/>
-      <c r="C17" s="279"/>
-      <c r="D17" s="279"/>
-      <c r="E17" s="279"/>
-      <c r="F17" s="279"/>
-      <c r="G17" s="279"/>
+      <c r="B17" s="285"/>
+      <c r="C17" s="285"/>
+      <c r="D17" s="285"/>
+      <c r="E17" s="285"/>
+      <c r="F17" s="285"/>
+      <c r="G17" s="285"/>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B18" s="279"/>
-      <c r="C18" s="279"/>
-      <c r="D18" s="279"/>
-      <c r="E18" s="279"/>
-      <c r="F18" s="279"/>
-      <c r="G18" s="279"/>
+      <c r="B18" s="285"/>
+      <c r="C18" s="285"/>
+      <c r="D18" s="285"/>
+      <c r="E18" s="285"/>
+      <c r="F18" s="285"/>
+      <c r="G18" s="285"/>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B19" s="279"/>
-      <c r="C19" s="279"/>
-      <c r="D19" s="279"/>
-      <c r="E19" s="279"/>
-      <c r="F19" s="279"/>
-      <c r="G19" s="279"/>
+      <c r="B19" s="285"/>
+      <c r="C19" s="285"/>
+      <c r="D19" s="285"/>
+      <c r="E19" s="285"/>
+      <c r="F19" s="285"/>
+      <c r="G19" s="285"/>
       <c r="I19" s="35"/>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B20" s="279"/>
-      <c r="C20" s="279"/>
-      <c r="D20" s="279"/>
-      <c r="E20" s="279"/>
-      <c r="F20" s="279"/>
-      <c r="G20" s="279"/>
+      <c r="B20" s="285"/>
+      <c r="C20" s="285"/>
+      <c r="D20" s="285"/>
+      <c r="E20" s="285"/>
+      <c r="F20" s="285"/>
+      <c r="G20" s="285"/>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B21" s="279"/>
-      <c r="C21" s="279"/>
-      <c r="D21" s="279"/>
-      <c r="E21" s="279"/>
-      <c r="F21" s="279"/>
-      <c r="G21" s="279"/>
+      <c r="B21" s="285"/>
+      <c r="C21" s="285"/>
+      <c r="D21" s="285"/>
+      <c r="E21" s="285"/>
+      <c r="F21" s="285"/>
+      <c r="G21" s="285"/>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B22" s="279"/>
-      <c r="C22" s="279"/>
-      <c r="D22" s="279"/>
-      <c r="E22" s="279"/>
-      <c r="F22" s="279"/>
-      <c r="G22" s="279"/>
+      <c r="B22" s="285"/>
+      <c r="C22" s="285"/>
+      <c r="D22" s="285"/>
+      <c r="E22" s="285"/>
+      <c r="F22" s="285"/>
+      <c r="G22" s="285"/>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B23" s="279"/>
-      <c r="C23" s="279"/>
-      <c r="D23" s="279"/>
-      <c r="E23" s="279"/>
-      <c r="F23" s="279"/>
-      <c r="G23" s="279"/>
+      <c r="B23" s="285"/>
+      <c r="C23" s="285"/>
+      <c r="D23" s="285"/>
+      <c r="E23" s="285"/>
+      <c r="F23" s="285"/>
+      <c r="G23" s="285"/>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B24" s="279"/>
-      <c r="C24" s="279"/>
-      <c r="D24" s="279"/>
-      <c r="E24" s="279"/>
-      <c r="F24" s="279"/>
-      <c r="G24" s="279"/>
+      <c r="B24" s="285"/>
+      <c r="C24" s="285"/>
+      <c r="D24" s="285"/>
+      <c r="E24" s="285"/>
+      <c r="F24" s="285"/>
+      <c r="G24" s="285"/>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B25" s="279"/>
-      <c r="C25" s="279"/>
-      <c r="D25" s="279"/>
-      <c r="E25" s="279"/>
-      <c r="F25" s="279"/>
-      <c r="G25" s="279"/>
+      <c r="B25" s="285"/>
+      <c r="C25" s="285"/>
+      <c r="D25" s="285"/>
+      <c r="E25" s="285"/>
+      <c r="F25" s="285"/>
+      <c r="G25" s="285"/>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B26" s="279"/>
-      <c r="C26" s="279"/>
-      <c r="D26" s="279"/>
-      <c r="E26" s="279"/>
-      <c r="F26" s="279"/>
-      <c r="G26" s="279"/>
+      <c r="B26" s="285"/>
+      <c r="C26" s="285"/>
+      <c r="D26" s="285"/>
+      <c r="E26" s="285"/>
+      <c r="F26" s="285"/>
+      <c r="G26" s="285"/>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B27" s="279"/>
-      <c r="C27" s="279"/>
-      <c r="D27" s="279"/>
-      <c r="E27" s="279"/>
-      <c r="F27" s="279"/>
-      <c r="G27" s="279"/>
+      <c r="B27" s="285"/>
+      <c r="C27" s="285"/>
+      <c r="D27" s="285"/>
+      <c r="E27" s="285"/>
+      <c r="F27" s="285"/>
+      <c r="G27" s="285"/>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B28" s="279"/>
-      <c r="C28" s="279"/>
-      <c r="D28" s="279"/>
-      <c r="E28" s="279"/>
-      <c r="F28" s="279"/>
-      <c r="G28" s="279"/>
+      <c r="B28" s="285"/>
+      <c r="C28" s="285"/>
+      <c r="D28" s="285"/>
+      <c r="E28" s="285"/>
+      <c r="F28" s="285"/>
+      <c r="G28" s="285"/>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B29" s="279"/>
-      <c r="C29" s="279"/>
-      <c r="D29" s="279"/>
-      <c r="E29" s="279"/>
-      <c r="F29" s="279"/>
-      <c r="G29" s="279"/>
+      <c r="B29" s="285"/>
+      <c r="C29" s="285"/>
+      <c r="D29" s="285"/>
+      <c r="E29" s="285"/>
+      <c r="F29" s="285"/>
+      <c r="G29" s="285"/>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B30" s="279"/>
-      <c r="C30" s="279"/>
-      <c r="D30" s="279"/>
-      <c r="E30" s="279"/>
-      <c r="F30" s="279"/>
-      <c r="G30" s="279"/>
+      <c r="B30" s="285"/>
+      <c r="C30" s="285"/>
+      <c r="D30" s="285"/>
+      <c r="E30" s="285"/>
+      <c r="F30" s="285"/>
+      <c r="G30" s="285"/>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B31" s="279"/>
-      <c r="C31" s="279"/>
-      <c r="D31" s="279"/>
-      <c r="E31" s="279"/>
-      <c r="F31" s="279"/>
-      <c r="G31" s="279"/>
+      <c r="B31" s="285"/>
+      <c r="C31" s="285"/>
+      <c r="D31" s="285"/>
+      <c r="E31" s="285"/>
+      <c r="F31" s="285"/>
+      <c r="G31" s="285"/>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B32" s="279"/>
-      <c r="C32" s="279"/>
-      <c r="D32" s="279"/>
-      <c r="E32" s="279"/>
-      <c r="F32" s="279"/>
-      <c r="G32" s="279"/>
+      <c r="B32" s="285"/>
+      <c r="C32" s="285"/>
+      <c r="D32" s="285"/>
+      <c r="E32" s="285"/>
+      <c r="F32" s="285"/>
+      <c r="G32" s="285"/>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B33" s="279"/>
-      <c r="C33" s="279"/>
-      <c r="D33" s="279"/>
-      <c r="E33" s="279"/>
-      <c r="F33" s="279"/>
-      <c r="G33" s="279"/>
+      <c r="B33" s="285"/>
+      <c r="C33" s="285"/>
+      <c r="D33" s="285"/>
+      <c r="E33" s="285"/>
+      <c r="F33" s="285"/>
+      <c r="G33" s="285"/>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B34" s="279"/>
-      <c r="C34" s="279"/>
-      <c r="D34" s="279"/>
-      <c r="E34" s="279"/>
-      <c r="F34" s="279"/>
-      <c r="G34" s="279"/>
+      <c r="B34" s="285"/>
+      <c r="C34" s="285"/>
+      <c r="D34" s="285"/>
+      <c r="E34" s="285"/>
+      <c r="F34" s="285"/>
+      <c r="G34" s="285"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B35" s="279"/>
-      <c r="C35" s="279"/>
-      <c r="D35" s="279"/>
-      <c r="E35" s="279"/>
-      <c r="F35" s="279"/>
-      <c r="G35" s="279"/>
+      <c r="B35" s="285"/>
+      <c r="C35" s="285"/>
+      <c r="D35" s="285"/>
+      <c r="E35" s="285"/>
+      <c r="F35" s="285"/>
+      <c r="G35" s="285"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B36" s="279"/>
-      <c r="C36" s="279"/>
-      <c r="D36" s="279"/>
-      <c r="E36" s="279"/>
-      <c r="F36" s="279"/>
-      <c r="G36" s="279"/>
+      <c r="B36" s="285"/>
+      <c r="C36" s="285"/>
+      <c r="D36" s="285"/>
+      <c r="E36" s="285"/>
+      <c r="F36" s="285"/>
+      <c r="G36" s="285"/>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B37" s="279"/>
-      <c r="C37" s="279"/>
-      <c r="D37" s="279"/>
-      <c r="E37" s="279"/>
-      <c r="F37" s="279"/>
-      <c r="G37" s="279"/>
+      <c r="B37" s="285"/>
+      <c r="C37" s="285"/>
+      <c r="D37" s="285"/>
+      <c r="E37" s="285"/>
+      <c r="F37" s="285"/>
+      <c r="G37" s="285"/>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B38" s="279"/>
-      <c r="C38" s="279"/>
-      <c r="D38" s="279"/>
-      <c r="E38" s="279"/>
-      <c r="F38" s="279"/>
-      <c r="G38" s="279"/>
+      <c r="B38" s="285"/>
+      <c r="C38" s="285"/>
+      <c r="D38" s="285"/>
+      <c r="E38" s="285"/>
+      <c r="F38" s="285"/>
+      <c r="G38" s="285"/>
     </row>
     <row r="41" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B41" s="30" t="str">
         <f ca="1">IF(LEN($E$9)&gt;1,"Datum: "&amp;IF(ISNUMBER(VALUE(TEXT(TODAY(),"rrrr"))),TEXT(TODAY(),"dd.mm.rrrr"),TEXT(TODAY(),"dd.mm.yyyy")),"Datum: ........................................")</f>
-        <v>Datum: 10.01.2019</v>
+        <v>Datum: 03.07.2019</v>
       </c>
       <c r="D41" s="30"/>
       <c r="E41" s="30"/>
@@ -7332,22 +7343,22 @@
       <c r="A4" s="156" t="s">
         <v>193</v>
       </c>
-      <c r="B4" s="273">
+      <c r="B4" s="279">
         <f>'Seznam účastníků'!B4</f>
         <v>0</v>
       </c>
-      <c r="C4" s="273"/>
+      <c r="C4" s="279"/>
       <c r="D4"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" s="156" t="s">
         <v>194</v>
       </c>
-      <c r="B5" s="274">
+      <c r="B5" s="280">
         <f>'Seznam účastníků'!B5</f>
         <v>0</v>
       </c>
-      <c r="C5" s="274"/>
+      <c r="C5" s="280"/>
       <c r="D5"/>
       <c r="E5" s="210"/>
     </row>
@@ -7355,11 +7366,11 @@
       <c r="A6" s="156" t="s">
         <v>195</v>
       </c>
-      <c r="B6" s="274">
+      <c r="B6" s="280">
         <f>'Seznam účastníků'!B6</f>
         <v>0</v>
       </c>
-      <c r="C6" s="274"/>
+      <c r="C6" s="280"/>
       <c r="D6"/>
       <c r="E6" s="210"/>
     </row>
@@ -7367,11 +7378,11 @@
       <c r="A7" s="156" t="s">
         <v>196</v>
       </c>
-      <c r="B7" s="273">
+      <c r="B7" s="279">
         <f>'Seznam účastníků'!B7</f>
         <v>0</v>
       </c>
-      <c r="C7" s="273"/>
+      <c r="C7" s="279"/>
       <c r="D7"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.2">
@@ -8572,18 +8583,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:256" s="34" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="223" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="223"/>
-      <c r="C1" s="223"/>
-      <c r="D1" s="223"/>
-      <c r="E1" s="223"/>
-      <c r="F1" s="223"/>
-      <c r="G1" s="223"/>
-      <c r="H1" s="223"/>
-      <c r="I1" s="223"/>
-      <c r="J1" s="223"/>
+      <c r="A1" s="245" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="245"/>
+      <c r="C1" s="245"/>
+      <c r="D1" s="245"/>
+      <c r="E1" s="245"/>
+      <c r="F1" s="245"/>
+      <c r="G1" s="245"/>
+      <c r="H1" s="245"/>
+      <c r="I1" s="245"/>
+      <c r="J1" s="245"/>
       <c r="IN1" s="35"/>
       <c r="IO1" s="35"/>
       <c r="IP1" s="35"/>
@@ -8596,15 +8607,15 @@
     </row>
     <row r="2" spans="1:256" s="34" customFormat="1" ht="29.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="36"/>
-      <c r="B2" s="218" t="s">
+      <c r="B2" s="223" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="218"/>
-      <c r="D2" s="218"/>
-      <c r="E2" s="218"/>
-      <c r="F2" s="218"/>
-      <c r="G2" s="218"/>
-      <c r="H2" s="218"/>
+      <c r="C2" s="223"/>
+      <c r="D2" s="223"/>
+      <c r="E2" s="223"/>
+      <c r="F2" s="223"/>
+      <c r="G2" s="223"/>
+      <c r="H2" s="223"/>
       <c r="I2" s="36"/>
       <c r="J2" s="36"/>
       <c r="IN2" s="35"/>
@@ -8660,17 +8671,17 @@
         <v>40</v>
       </c>
       <c r="C7" s="6"/>
-      <c r="D7" s="224" t="s">
+      <c r="D7" s="246" t="s">
         <v>41</v>
       </c>
-      <c r="E7" s="224"/>
+      <c r="E7" s="246"/>
       <c r="F7" s="37"/>
-      <c r="G7" s="225" t="s">
+      <c r="G7" s="247" t="s">
         <v>42</v>
       </c>
-      <c r="H7" s="225"/>
-      <c r="I7" s="225"/>
-      <c r="J7" s="225"/>
+      <c r="H7" s="247"/>
+      <c r="I7" s="247"/>
+      <c r="J7" s="247"/>
     </row>
     <row r="8" spans="1:256" x14ac:dyDescent="0.2">
       <c r="A8" s="6"/>
@@ -8679,19 +8690,19 @@
         <v>Šán</v>
       </c>
       <c r="C8" s="6"/>
-      <c r="D8" s="226" t="str">
+      <c r="D8" s="248" t="str">
         <f ca="1">IF(AND(ISNUMBER('Seznam účastníků'!B5),ISNUMBER('Seznam účastníků'!B6)),IF(ISNUMBER(VALUE(TEXT(TODAY(),"rrrr"))),TEXT('Seznam účastníků'!B5,"dd.mm.rrrr")&amp;" - "&amp;TEXT('Seznam účastníků'!B6,"dd.mm.rrrr"),TEXT('Seznam účastníků'!B5,"dd.mm.yyyy")&amp;" - "&amp;TEXT('Seznam účastníků'!B6,"dd.mm.yyyy"))," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E8" s="226"/>
+      <c r="E8" s="248"/>
       <c r="F8" s="35"/>
-      <c r="G8" s="227">
+      <c r="G8" s="249">
         <f>IF(ISBLANK(Seznam_do_35_účastníků!C6),IF(ISBLANK(Seznam_do_70_účastníků!C6)," ",Seznam_do_70_účastníků!C6),Seznam_do_35_účastníků!C6)</f>
         <v>0</v>
       </c>
-      <c r="H8" s="227"/>
-      <c r="I8" s="227"/>
-      <c r="J8" s="227"/>
+      <c r="H8" s="249"/>
+      <c r="I8" s="249"/>
+      <c r="J8" s="249"/>
     </row>
     <row r="9" spans="1:256" x14ac:dyDescent="0.2">
       <c r="A9" s="6"/>
@@ -8757,340 +8768,340 @@
       <c r="B14" s="51" t="s">
         <v>46</v>
       </c>
-      <c r="C14" s="228" t="s">
+      <c r="C14" s="239" t="s">
         <v>47</v>
       </c>
-      <c r="D14" s="228"/>
-      <c r="E14" s="229" t="s">
+      <c r="D14" s="239"/>
+      <c r="E14" s="240" t="s">
         <v>48</v>
       </c>
-      <c r="F14" s="229"/>
-      <c r="G14" s="229"/>
+      <c r="F14" s="240"/>
+      <c r="G14" s="240"/>
       <c r="H14" s="52"/>
-      <c r="I14" s="230" t="s">
+      <c r="I14" s="241" t="s">
         <v>49</v>
       </c>
-      <c r="J14" s="230"/>
+      <c r="J14" s="241"/>
     </row>
     <row r="15" spans="1:256" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
       <c r="B15" s="53" t="s">
         <v>50</v>
       </c>
-      <c r="C15" s="231">
+      <c r="C15" s="242">
         <v>40179</v>
       </c>
-      <c r="D15" s="231"/>
-      <c r="E15" s="232" t="s">
+      <c r="D15" s="242"/>
+      <c r="E15" s="243" t="s">
         <v>51</v>
       </c>
-      <c r="F15" s="232"/>
-      <c r="G15" s="232"/>
+      <c r="F15" s="243"/>
+      <c r="G15" s="243"/>
       <c r="H15" s="54"/>
-      <c r="I15" s="233">
+      <c r="I15" s="244">
         <v>100</v>
       </c>
-      <c r="J15" s="233"/>
+      <c r="J15" s="244"/>
     </row>
     <row r="16" spans="1:256" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
       <c r="B16" s="55"/>
-      <c r="C16" s="234"/>
-      <c r="D16" s="234"/>
-      <c r="E16" s="235" t="s">
+      <c r="C16" s="238"/>
+      <c r="D16" s="238"/>
+      <c r="E16" s="232" t="s">
         <v>52</v>
       </c>
-      <c r="F16" s="235"/>
-      <c r="G16" s="235"/>
+      <c r="F16" s="232"/>
+      <c r="G16" s="232"/>
       <c r="H16" s="54"/>
-      <c r="I16" s="236">
+      <c r="I16" s="233">
         <v>3042</v>
       </c>
-      <c r="J16" s="236"/>
+      <c r="J16" s="233"/>
     </row>
     <row r="17" spans="1:10" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
       <c r="B17" s="53"/>
       <c r="C17" s="237"/>
       <c r="D17" s="237"/>
-      <c r="E17" s="235"/>
-      <c r="F17" s="235"/>
-      <c r="G17" s="235"/>
+      <c r="E17" s="232"/>
+      <c r="F17" s="232"/>
+      <c r="G17" s="232"/>
       <c r="H17" s="54"/>
-      <c r="I17" s="236"/>
-      <c r="J17" s="236"/>
+      <c r="I17" s="233"/>
+      <c r="J17" s="233"/>
     </row>
     <row r="18" spans="1:10" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
       <c r="B18" s="53"/>
       <c r="C18" s="237"/>
       <c r="D18" s="237"/>
-      <c r="E18" s="235"/>
-      <c r="F18" s="235"/>
-      <c r="G18" s="235"/>
+      <c r="E18" s="232"/>
+      <c r="F18" s="232"/>
+      <c r="G18" s="232"/>
       <c r="H18" s="54"/>
-      <c r="I18" s="236"/>
-      <c r="J18" s="236"/>
+      <c r="I18" s="233"/>
+      <c r="J18" s="233"/>
     </row>
     <row r="19" spans="1:10" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
       <c r="B19" s="53"/>
       <c r="C19" s="237"/>
       <c r="D19" s="237"/>
-      <c r="E19" s="235"/>
-      <c r="F19" s="235"/>
-      <c r="G19" s="235"/>
+      <c r="E19" s="232"/>
+      <c r="F19" s="232"/>
+      <c r="G19" s="232"/>
       <c r="H19" s="54"/>
-      <c r="I19" s="236"/>
-      <c r="J19" s="236"/>
+      <c r="I19" s="233"/>
+      <c r="J19" s="233"/>
     </row>
     <row r="20" spans="1:10" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
       <c r="B20" s="53"/>
       <c r="C20" s="237"/>
       <c r="D20" s="237"/>
-      <c r="E20" s="235"/>
-      <c r="F20" s="235"/>
-      <c r="G20" s="235"/>
+      <c r="E20" s="232"/>
+      <c r="F20" s="232"/>
+      <c r="G20" s="232"/>
       <c r="H20" s="54"/>
-      <c r="I20" s="236"/>
-      <c r="J20" s="236"/>
+      <c r="I20" s="233"/>
+      <c r="J20" s="233"/>
     </row>
     <row r="21" spans="1:10" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
       <c r="B21" s="53"/>
-      <c r="C21" s="238"/>
-      <c r="D21" s="238"/>
-      <c r="E21" s="235"/>
-      <c r="F21" s="235"/>
-      <c r="G21" s="235"/>
+      <c r="C21" s="236"/>
+      <c r="D21" s="236"/>
+      <c r="E21" s="232"/>
+      <c r="F21" s="232"/>
+      <c r="G21" s="232"/>
       <c r="H21" s="54"/>
-      <c r="I21" s="236"/>
-      <c r="J21" s="236"/>
+      <c r="I21" s="233"/>
+      <c r="J21" s="233"/>
     </row>
     <row r="22" spans="1:10" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="6"/>
       <c r="B22" s="53"/>
-      <c r="C22" s="238"/>
-      <c r="D22" s="238"/>
-      <c r="E22" s="235"/>
-      <c r="F22" s="235"/>
-      <c r="G22" s="235"/>
+      <c r="C22" s="236"/>
+      <c r="D22" s="236"/>
+      <c r="E22" s="232"/>
+      <c r="F22" s="232"/>
+      <c r="G22" s="232"/>
       <c r="H22" s="54"/>
-      <c r="I22" s="236"/>
-      <c r="J22" s="236"/>
+      <c r="I22" s="233"/>
+      <c r="J22" s="233"/>
     </row>
     <row r="23" spans="1:10" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="6"/>
       <c r="B23" s="53"/>
-      <c r="C23" s="238"/>
-      <c r="D23" s="238"/>
-      <c r="E23" s="235"/>
-      <c r="F23" s="235"/>
-      <c r="G23" s="235"/>
+      <c r="C23" s="236"/>
+      <c r="D23" s="236"/>
+      <c r="E23" s="232"/>
+      <c r="F23" s="232"/>
+      <c r="G23" s="232"/>
       <c r="H23" s="54"/>
-      <c r="I23" s="236"/>
-      <c r="J23" s="236"/>
+      <c r="I23" s="233"/>
+      <c r="J23" s="233"/>
     </row>
     <row r="24" spans="1:10" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="6"/>
       <c r="B24" s="53"/>
-      <c r="C24" s="238"/>
-      <c r="D24" s="238"/>
-      <c r="E24" s="235"/>
-      <c r="F24" s="235"/>
-      <c r="G24" s="235"/>
+      <c r="C24" s="236"/>
+      <c r="D24" s="236"/>
+      <c r="E24" s="232"/>
+      <c r="F24" s="232"/>
+      <c r="G24" s="232"/>
       <c r="H24" s="54"/>
-      <c r="I24" s="236"/>
-      <c r="J24" s="236"/>
+      <c r="I24" s="233"/>
+      <c r="J24" s="233"/>
     </row>
     <row r="25" spans="1:10" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="6"/>
       <c r="B25" s="53"/>
-      <c r="C25" s="238"/>
-      <c r="D25" s="238"/>
-      <c r="E25" s="235"/>
-      <c r="F25" s="235"/>
-      <c r="G25" s="235"/>
+      <c r="C25" s="236"/>
+      <c r="D25" s="236"/>
+      <c r="E25" s="232"/>
+      <c r="F25" s="232"/>
+      <c r="G25" s="232"/>
       <c r="H25" s="54"/>
-      <c r="I25" s="236"/>
-      <c r="J25" s="236"/>
+      <c r="I25" s="233"/>
+      <c r="J25" s="233"/>
     </row>
     <row r="26" spans="1:10" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="6"/>
       <c r="B26" s="53"/>
-      <c r="C26" s="238"/>
-      <c r="D26" s="238"/>
-      <c r="E26" s="235"/>
-      <c r="F26" s="235"/>
-      <c r="G26" s="235"/>
+      <c r="C26" s="236"/>
+      <c r="D26" s="236"/>
+      <c r="E26" s="232"/>
+      <c r="F26" s="232"/>
+      <c r="G26" s="232"/>
       <c r="H26" s="54"/>
-      <c r="I26" s="236"/>
-      <c r="J26" s="236"/>
+      <c r="I26" s="233"/>
+      <c r="J26" s="233"/>
     </row>
     <row r="27" spans="1:10" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="6"/>
       <c r="B27" s="56"/>
-      <c r="C27" s="239"/>
-      <c r="D27" s="239"/>
-      <c r="E27" s="235"/>
-      <c r="F27" s="235"/>
-      <c r="G27" s="235"/>
+      <c r="C27" s="231"/>
+      <c r="D27" s="231"/>
+      <c r="E27" s="232"/>
+      <c r="F27" s="232"/>
+      <c r="G27" s="232"/>
       <c r="H27" s="54"/>
-      <c r="I27" s="236"/>
-      <c r="J27" s="236"/>
+      <c r="I27" s="233"/>
+      <c r="J27" s="233"/>
     </row>
     <row r="28" spans="1:10" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="6"/>
       <c r="B28" s="56"/>
-      <c r="C28" s="239"/>
-      <c r="D28" s="239"/>
-      <c r="E28" s="235"/>
-      <c r="F28" s="235"/>
-      <c r="G28" s="235"/>
+      <c r="C28" s="231"/>
+      <c r="D28" s="231"/>
+      <c r="E28" s="232"/>
+      <c r="F28" s="232"/>
+      <c r="G28" s="232"/>
       <c r="H28" s="54"/>
-      <c r="I28" s="236"/>
-      <c r="J28" s="236"/>
+      <c r="I28" s="233"/>
+      <c r="J28" s="233"/>
     </row>
     <row r="29" spans="1:10" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>
       <c r="B29" s="56"/>
-      <c r="C29" s="239"/>
-      <c r="D29" s="239"/>
-      <c r="E29" s="235"/>
-      <c r="F29" s="235"/>
-      <c r="G29" s="235"/>
+      <c r="C29" s="231"/>
+      <c r="D29" s="231"/>
+      <c r="E29" s="232"/>
+      <c r="F29" s="232"/>
+      <c r="G29" s="232"/>
       <c r="H29" s="54"/>
-      <c r="I29" s="236"/>
-      <c r="J29" s="236"/>
+      <c r="I29" s="233"/>
+      <c r="J29" s="233"/>
     </row>
     <row r="30" spans="1:10" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="6"/>
       <c r="B30" s="56"/>
-      <c r="C30" s="239"/>
-      <c r="D30" s="239"/>
-      <c r="E30" s="235"/>
-      <c r="F30" s="235"/>
-      <c r="G30" s="235"/>
+      <c r="C30" s="231"/>
+      <c r="D30" s="231"/>
+      <c r="E30" s="232"/>
+      <c r="F30" s="232"/>
+      <c r="G30" s="232"/>
       <c r="H30" s="54"/>
-      <c r="I30" s="236"/>
-      <c r="J30" s="236"/>
+      <c r="I30" s="233"/>
+      <c r="J30" s="233"/>
     </row>
     <row r="31" spans="1:10" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="6"/>
       <c r="B31" s="56"/>
-      <c r="C31" s="239"/>
-      <c r="D31" s="239"/>
-      <c r="E31" s="235"/>
-      <c r="F31" s="235"/>
-      <c r="G31" s="235"/>
+      <c r="C31" s="231"/>
+      <c r="D31" s="231"/>
+      <c r="E31" s="232"/>
+      <c r="F31" s="232"/>
+      <c r="G31" s="232"/>
       <c r="H31" s="54"/>
-      <c r="I31" s="236"/>
-      <c r="J31" s="236"/>
+      <c r="I31" s="233"/>
+      <c r="J31" s="233"/>
     </row>
     <row r="32" spans="1:10" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="6"/>
       <c r="B32" s="56"/>
-      <c r="C32" s="239"/>
-      <c r="D32" s="239"/>
-      <c r="E32" s="235"/>
-      <c r="F32" s="235"/>
-      <c r="G32" s="235"/>
+      <c r="C32" s="231"/>
+      <c r="D32" s="231"/>
+      <c r="E32" s="232"/>
+      <c r="F32" s="232"/>
+      <c r="G32" s="232"/>
       <c r="H32" s="54"/>
-      <c r="I32" s="236"/>
-      <c r="J32" s="236"/>
+      <c r="I32" s="233"/>
+      <c r="J32" s="233"/>
     </row>
     <row r="33" spans="1:10" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="6"/>
       <c r="B33" s="56"/>
-      <c r="C33" s="239"/>
-      <c r="D33" s="239"/>
-      <c r="E33" s="235"/>
-      <c r="F33" s="235"/>
-      <c r="G33" s="235"/>
+      <c r="C33" s="231"/>
+      <c r="D33" s="231"/>
+      <c r="E33" s="232"/>
+      <c r="F33" s="232"/>
+      <c r="G33" s="232"/>
       <c r="H33" s="54"/>
-      <c r="I33" s="236"/>
-      <c r="J33" s="236"/>
+      <c r="I33" s="233"/>
+      <c r="J33" s="233"/>
     </row>
     <row r="34" spans="1:10" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="6"/>
       <c r="B34" s="56"/>
-      <c r="C34" s="239"/>
-      <c r="D34" s="239"/>
-      <c r="E34" s="235"/>
-      <c r="F34" s="235"/>
-      <c r="G34" s="235"/>
+      <c r="C34" s="231"/>
+      <c r="D34" s="231"/>
+      <c r="E34" s="232"/>
+      <c r="F34" s="232"/>
+      <c r="G34" s="232"/>
       <c r="H34" s="54"/>
-      <c r="I34" s="236"/>
-      <c r="J34" s="236"/>
+      <c r="I34" s="233"/>
+      <c r="J34" s="233"/>
     </row>
     <row r="35" spans="1:10" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="6"/>
       <c r="B35" s="56"/>
-      <c r="C35" s="239"/>
-      <c r="D35" s="239"/>
-      <c r="E35" s="235"/>
-      <c r="F35" s="235"/>
-      <c r="G35" s="235"/>
+      <c r="C35" s="231"/>
+      <c r="D35" s="231"/>
+      <c r="E35" s="232"/>
+      <c r="F35" s="232"/>
+      <c r="G35" s="232"/>
       <c r="H35" s="54"/>
-      <c r="I35" s="236"/>
-      <c r="J35" s="236"/>
+      <c r="I35" s="233"/>
+      <c r="J35" s="233"/>
     </row>
     <row r="36" spans="1:10" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="6"/>
       <c r="B36" s="56"/>
-      <c r="C36" s="239"/>
-      <c r="D36" s="239"/>
-      <c r="E36" s="235"/>
-      <c r="F36" s="235"/>
-      <c r="G36" s="235"/>
+      <c r="C36" s="231"/>
+      <c r="D36" s="231"/>
+      <c r="E36" s="232"/>
+      <c r="F36" s="232"/>
+      <c r="G36" s="232"/>
       <c r="H36" s="54"/>
-      <c r="I36" s="236"/>
-      <c r="J36" s="236"/>
+      <c r="I36" s="233"/>
+      <c r="J36" s="233"/>
     </row>
     <row r="37" spans="1:10" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="6"/>
       <c r="B37" s="56"/>
-      <c r="C37" s="239"/>
-      <c r="D37" s="239"/>
-      <c r="E37" s="235"/>
-      <c r="F37" s="235"/>
-      <c r="G37" s="235"/>
+      <c r="C37" s="231"/>
+      <c r="D37" s="231"/>
+      <c r="E37" s="232"/>
+      <c r="F37" s="232"/>
+      <c r="G37" s="232"/>
       <c r="H37" s="54"/>
-      <c r="I37" s="236"/>
-      <c r="J37" s="236"/>
+      <c r="I37" s="233"/>
+      <c r="J37" s="233"/>
     </row>
     <row r="38" spans="1:10" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="6"/>
       <c r="B38" s="56"/>
-      <c r="C38" s="239"/>
-      <c r="D38" s="239"/>
-      <c r="E38" s="235"/>
-      <c r="F38" s="235"/>
-      <c r="G38" s="235"/>
+      <c r="C38" s="231"/>
+      <c r="D38" s="231"/>
+      <c r="E38" s="232"/>
+      <c r="F38" s="232"/>
+      <c r="G38" s="232"/>
       <c r="H38" s="54"/>
-      <c r="I38" s="236"/>
-      <c r="J38" s="236"/>
+      <c r="I38" s="233"/>
+      <c r="J38" s="233"/>
     </row>
     <row r="39" spans="1:10" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="6"/>
       <c r="B39" s="56"/>
-      <c r="C39" s="243"/>
-      <c r="D39" s="243"/>
-      <c r="E39" s="244"/>
-      <c r="F39" s="244"/>
-      <c r="G39" s="244"/>
+      <c r="C39" s="234"/>
+      <c r="D39" s="234"/>
+      <c r="E39" s="235"/>
+      <c r="F39" s="235"/>
+      <c r="G39" s="235"/>
       <c r="H39" s="57"/>
-      <c r="I39" s="236"/>
-      <c r="J39" s="236"/>
+      <c r="I39" s="233"/>
+      <c r="J39" s="233"/>
     </row>
     <row r="40" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="6"/>
-      <c r="B40" s="240" t="s">
+      <c r="B40" s="228" t="s">
         <v>53</v>
       </c>
-      <c r="C40" s="240"/>
-      <c r="D40" s="240"/>
+      <c r="C40" s="228"/>
+      <c r="D40" s="228"/>
       <c r="F40" s="58">
         <f>IF(AND(ISNUMBER('Seznam účastníků'!B5),ISNUMBER('Seznam účastníků'!B6)),('Seznam účastníků'!B6-'Seznam účastníků'!B5+1),0)</f>
         <v>0</v>
@@ -9100,11 +9111,11 @@
         <v>#VALUE!</v>
       </c>
       <c r="H40" s="34"/>
-      <c r="I40" s="241">
+      <c r="I40" s="229">
         <f>SUM(I15:J39)</f>
         <v>3142</v>
       </c>
-      <c r="J40" s="241"/>
+      <c r="J40" s="229"/>
     </row>
     <row r="41" spans="1:10" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="31" t="s">
@@ -9121,10 +9132,10 @@
         <v>#VALUE!</v>
       </c>
       <c r="H41" s="27"/>
-      <c r="I41" s="242">
+      <c r="I41" s="230">
         <v>100</v>
       </c>
-      <c r="J41" s="242"/>
+      <c r="J41" s="230"/>
     </row>
     <row r="42" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="29"/>
@@ -9132,10 +9143,10 @@
         <v>55</v>
       </c>
       <c r="E42" s="35"/>
-      <c r="I42" s="242">
+      <c r="I42" s="230">
         <v>160</v>
       </c>
-      <c r="J42" s="242"/>
+      <c r="J42" s="230"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="E43" s="1" t="e">
@@ -9146,7 +9157,7 @@
     <row r="45" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B45" s="30" t="str">
         <f ca="1">IF($B$15&lt;&gt;"","Datum: "&amp;IF(ISNUMBER(VALUE(TEXT(TODAY(),"rrrr"))),TEXT(TODAY(),"dd.mm.rrrr"),TEXT(TODAY(),"dd.mm.yyyy")),"Datum: ........................................")</f>
-        <v>Datum: 10.01.2019</v>
+        <v>Datum: 03.07.2019</v>
       </c>
       <c r="C45" s="30"/>
       <c r="D45" s="30"/>
@@ -9169,6 +9180,84 @@
   </sheetData>
   <sheetProtection sheet="1"/>
   <mergeCells count="88">
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="G7:J7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="G8:J8"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="E19:G19"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="E20:G20"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="E21:G21"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="E22:G22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="E27:G27"/>
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="E29:G29"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="E30:G30"/>
+    <mergeCell ref="I30:J30"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="E31:G31"/>
+    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="E32:G32"/>
+    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="E33:G33"/>
+    <mergeCell ref="I33:J33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="E34:G34"/>
+    <mergeCell ref="I34:J34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="I35:J35"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="I36:J36"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="I37:J37"/>
     <mergeCell ref="B40:D40"/>
     <mergeCell ref="I40:J40"/>
     <mergeCell ref="I41:J41"/>
@@ -9179,84 +9268,6 @@
     <mergeCell ref="C39:D39"/>
     <mergeCell ref="E39:G39"/>
     <mergeCell ref="I39:J39"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="I36:J36"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="E37:G37"/>
-    <mergeCell ref="I37:J37"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="E34:G34"/>
-    <mergeCell ref="I34:J34"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="E35:G35"/>
-    <mergeCell ref="I35:J35"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="E32:G32"/>
-    <mergeCell ref="I32:J32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="E33:G33"/>
-    <mergeCell ref="I33:J33"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="E30:G30"/>
-    <mergeCell ref="I30:J30"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="E31:G31"/>
-    <mergeCell ref="I31:J31"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="I28:J28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="E29:G29"/>
-    <mergeCell ref="I29:J29"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="E27:G27"/>
-    <mergeCell ref="I27:J27"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="I24:J24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="E25:G25"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="E22:G22"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="E20:G20"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="E21:G21"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="E18:G18"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="E19:G19"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="E17:G17"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="E15:G15"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="G7:J7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="G8:J8"/>
   </mergeCells>
   <conditionalFormatting sqref="I41">
     <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">
@@ -9293,14 +9304,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:256" s="60" customFormat="1" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A1" s="245" t="s">
+      <c r="A1" s="250" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="245"/>
-      <c r="C1" s="245"/>
-      <c r="D1" s="245"/>
-      <c r="E1" s="245"/>
-      <c r="F1" s="245"/>
+      <c r="B1" s="250"/>
+      <c r="C1" s="250"/>
+      <c r="D1" s="250"/>
+      <c r="E1" s="250"/>
+      <c r="F1" s="250"/>
       <c r="IU1"/>
       <c r="IV1"/>
     </row>
@@ -11163,14 +11174,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:256" s="60" customFormat="1" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A1" s="245" t="s">
+      <c r="A1" s="250" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="245"/>
-      <c r="C1" s="245"/>
-      <c r="D1" s="245"/>
-      <c r="E1" s="245"/>
-      <c r="F1" s="245"/>
+      <c r="B1" s="250"/>
+      <c r="C1" s="250"/>
+      <c r="D1" s="250"/>
+      <c r="E1" s="250"/>
+      <c r="F1" s="250"/>
       <c r="IV1"/>
     </row>
     <row r="2" spans="1:256" s="60" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -12959,18 +12970,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:256" s="90" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A1" s="248" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="248"/>
-      <c r="C1" s="248"/>
-      <c r="D1" s="248"/>
-      <c r="E1" s="248"/>
-      <c r="F1" s="248"/>
-      <c r="G1" s="248"/>
-      <c r="H1" s="248"/>
-      <c r="I1" s="248"/>
-      <c r="J1" s="248"/>
+      <c r="A1" s="260" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="260"/>
+      <c r="C1" s="260"/>
+      <c r="D1" s="260"/>
+      <c r="E1" s="260"/>
+      <c r="F1" s="260"/>
+      <c r="G1" s="260"/>
+      <c r="H1" s="260"/>
+      <c r="I1" s="260"/>
+      <c r="J1" s="260"/>
       <c r="K1" s="89"/>
       <c r="L1" s="89"/>
       <c r="M1" s="89"/>
@@ -12991,20 +13002,20 @@
       <c r="IV1" s="89"/>
     </row>
     <row r="2" spans="1:256" s="90" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="249" t="str">
+      <c r="A2" s="261" t="str">
         <f>'Formulář  AKCE'!B2</f>
         <v>smlouvy č. DAG/61/03/001435/2009 o poskytnutí finančních prostředků
 Příloha k vyúčtování akcí a táborů</v>
       </c>
-      <c r="B2" s="249"/>
-      <c r="C2" s="249"/>
-      <c r="D2" s="249"/>
-      <c r="E2" s="249"/>
-      <c r="F2" s="249"/>
-      <c r="G2" s="249"/>
-      <c r="H2" s="249"/>
-      <c r="I2" s="249"/>
-      <c r="J2" s="249"/>
+      <c r="B2" s="261"/>
+      <c r="C2" s="261"/>
+      <c r="D2" s="261"/>
+      <c r="E2" s="261"/>
+      <c r="F2" s="261"/>
+      <c r="G2" s="261"/>
+      <c r="H2" s="261"/>
+      <c r="I2" s="261"/>
+      <c r="J2" s="261"/>
       <c r="K2" s="89"/>
       <c r="L2" s="89"/>
       <c r="M2" s="89"/>
@@ -13067,17 +13078,17 @@
         <v>40</v>
       </c>
       <c r="C7" s="92"/>
-      <c r="D7" s="250" t="s">
+      <c r="D7" s="262" t="s">
         <v>41</v>
       </c>
-      <c r="E7" s="250"/>
+      <c r="E7" s="262"/>
       <c r="F7" s="91"/>
-      <c r="G7" s="251" t="s">
+      <c r="G7" s="263" t="s">
         <v>42</v>
       </c>
-      <c r="H7" s="251"/>
-      <c r="I7" s="251"/>
-      <c r="J7" s="251"/>
+      <c r="H7" s="263"/>
+      <c r="I7" s="263"/>
+      <c r="J7" s="263"/>
     </row>
     <row r="8" spans="1:256" x14ac:dyDescent="0.2">
       <c r="A8" s="92"/>
@@ -13086,19 +13097,19 @@
         <v>Šán</v>
       </c>
       <c r="C8" s="92"/>
-      <c r="D8" s="252" t="str">
+      <c r="D8" s="264" t="str">
         <f ca="1">IF(AND(ISNUMBER('Seznam účastníků'!B5),ISNUMBER('Seznam účastníků'!B6)),IF(ISNUMBER(VALUE(TEXT(TODAY(),"rrrr"))),TEXT('Seznam účastníků'!B5,"dd.mm.rrrr")&amp;" - "&amp;TEXT('Seznam účastníků'!B6,"dd.mm.rrrr"),TEXT('Seznam účastníků'!B5,"dd.mm.yyyy")&amp;" - "&amp;TEXT('Seznam účastníků'!B6,"dd.mm.yyyy"))," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E8" s="252"/>
+      <c r="E8" s="264"/>
       <c r="F8" s="89"/>
-      <c r="G8" s="253">
+      <c r="G8" s="265">
         <f>IF(ISBLANK(Seznam_do_35_účastníků!C6),IF(ISBLANK(Seznam_do_70_účastníků!C6)," ",Seznam_do_70_účastníků!C6),Seznam_do_35_účastníků!C6)</f>
         <v>0</v>
       </c>
-      <c r="H8" s="253"/>
-      <c r="I8" s="253"/>
-      <c r="J8" s="253"/>
+      <c r="H8" s="265"/>
+      <c r="I8" s="265"/>
+      <c r="J8" s="265"/>
     </row>
     <row r="9" spans="1:256" x14ac:dyDescent="0.2">
       <c r="A9" s="92"/>
@@ -13157,18 +13168,18 @@
       <c r="J12" s="89"/>
     </row>
     <row r="13" spans="1:256" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="254" t="s">
+      <c r="A13" s="266" t="s">
         <v>130</v>
       </c>
-      <c r="B13" s="254"/>
-      <c r="C13" s="254"/>
-      <c r="D13" s="254"/>
-      <c r="E13" s="254"/>
-      <c r="F13" s="254"/>
-      <c r="G13" s="254"/>
-      <c r="H13" s="254"/>
-      <c r="I13" s="254"/>
-      <c r="J13" s="254"/>
+      <c r="B13" s="266"/>
+      <c r="C13" s="266"/>
+      <c r="D13" s="266"/>
+      <c r="E13" s="266"/>
+      <c r="F13" s="266"/>
+      <c r="G13" s="266"/>
+      <c r="H13" s="266"/>
+      <c r="I13" s="266"/>
+      <c r="J13" s="266"/>
     </row>
     <row r="14" spans="1:256" x14ac:dyDescent="0.2">
       <c r="A14" s="92"/>
@@ -13184,91 +13195,91 @@
     </row>
     <row r="15" spans="1:256" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="92"/>
-      <c r="B15" s="255" t="s">
+      <c r="B15" s="257" t="s">
         <v>131</v>
       </c>
-      <c r="C15" s="255"/>
-      <c r="D15" s="255"/>
-      <c r="E15" s="255"/>
-      <c r="F15" s="255"/>
+      <c r="C15" s="257"/>
+      <c r="D15" s="257"/>
+      <c r="E15" s="257"/>
+      <c r="F15" s="257"/>
       <c r="G15" s="102" t="s">
         <v>132</v>
       </c>
-      <c r="H15" s="256" t="s">
+      <c r="H15" s="258" t="s">
         <v>133</v>
       </c>
-      <c r="I15" s="256"/>
+      <c r="I15" s="258"/>
       <c r="J15" s="103"/>
     </row>
     <row r="16" spans="1:256" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="92"/>
-      <c r="B16" s="246" t="s">
+      <c r="B16" s="254" t="s">
         <v>134</v>
       </c>
-      <c r="C16" s="246"/>
-      <c r="D16" s="246"/>
-      <c r="E16" s="246"/>
-      <c r="F16" s="246"/>
+      <c r="C16" s="254"/>
+      <c r="D16" s="254"/>
+      <c r="E16" s="254"/>
+      <c r="F16" s="254"/>
       <c r="G16" s="104">
         <f>'Přehled o vybraných poplatcích'!E49</f>
         <v>0</v>
       </c>
-      <c r="H16" s="247"/>
-      <c r="I16" s="247"/>
+      <c r="H16" s="259"/>
+      <c r="I16" s="259"/>
       <c r="J16" s="103"/>
     </row>
     <row r="17" spans="1:10" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="92"/>
-      <c r="B17" s="246" t="s">
+      <c r="B17" s="254" t="s">
         <v>135</v>
       </c>
-      <c r="C17" s="246"/>
-      <c r="D17" s="246"/>
-      <c r="E17" s="246"/>
-      <c r="F17" s="246"/>
+      <c r="C17" s="254"/>
+      <c r="D17" s="254"/>
+      <c r="E17" s="254"/>
+      <c r="F17" s="254"/>
       <c r="G17" s="105">
         <v>0</v>
       </c>
-      <c r="H17" s="247">
+      <c r="H17" s="259">
         <v>1000</v>
       </c>
-      <c r="I17" s="247"/>
+      <c r="I17" s="259"/>
       <c r="J17" s="103"/>
     </row>
     <row r="18" spans="1:10" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="92"/>
-      <c r="B18" s="246" t="s">
+      <c r="B18" s="254" t="s">
         <v>136</v>
       </c>
-      <c r="C18" s="246"/>
-      <c r="D18" s="246"/>
-      <c r="E18" s="246"/>
-      <c r="F18" s="246"/>
+      <c r="C18" s="254"/>
+      <c r="D18" s="254"/>
+      <c r="E18" s="254"/>
+      <c r="F18" s="254"/>
       <c r="G18" s="105">
         <v>62</v>
       </c>
-      <c r="H18" s="257"/>
-      <c r="I18" s="257"/>
+      <c r="H18" s="255"/>
+      <c r="I18" s="255"/>
       <c r="J18" s="103"/>
     </row>
     <row r="19" spans="1:10" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="92"/>
-      <c r="B19" s="246" t="s">
+      <c r="B19" s="254" t="s">
         <v>137</v>
       </c>
-      <c r="C19" s="246"/>
-      <c r="D19" s="246"/>
-      <c r="E19" s="246"/>
-      <c r="F19" s="246"/>
+      <c r="C19" s="254"/>
+      <c r="D19" s="254"/>
+      <c r="E19" s="254"/>
+      <c r="F19" s="254"/>
       <c r="G19" s="104">
         <f>SUM(G16:G18)</f>
         <v>62</v>
       </c>
-      <c r="H19" s="258">
+      <c r="H19" s="256">
         <f>SUM(H17:I18)</f>
         <v>1000</v>
       </c>
-      <c r="I19" s="258"/>
+      <c r="I19" s="256"/>
       <c r="J19" s="106">
         <f>G19+H19</f>
         <v>1062</v>
@@ -13288,118 +13299,118 @@
     </row>
     <row r="21" spans="1:10" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="92"/>
-      <c r="B21" s="255" t="s">
+      <c r="B21" s="257" t="s">
         <v>138</v>
       </c>
-      <c r="C21" s="255"/>
-      <c r="D21" s="255"/>
-      <c r="E21" s="255"/>
-      <c r="F21" s="255"/>
+      <c r="C21" s="257"/>
+      <c r="D21" s="257"/>
+      <c r="E21" s="257"/>
+      <c r="F21" s="257"/>
       <c r="G21" s="109" t="s">
         <v>132</v>
       </c>
-      <c r="H21" s="256" t="s">
+      <c r="H21" s="258" t="s">
         <v>139</v>
       </c>
-      <c r="I21" s="256"/>
+      <c r="I21" s="258"/>
       <c r="J21" s="103"/>
     </row>
     <row r="22" spans="1:10" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="92"/>
-      <c r="B22" s="259" t="s">
+      <c r="B22" s="251" t="s">
         <v>140</v>
       </c>
-      <c r="C22" s="259"/>
-      <c r="D22" s="259"/>
-      <c r="E22" s="259"/>
-      <c r="F22" s="259"/>
+      <c r="C22" s="251"/>
+      <c r="D22" s="251"/>
+      <c r="E22" s="251"/>
+      <c r="F22" s="251"/>
       <c r="G22" s="105">
         <v>1000</v>
       </c>
-      <c r="H22" s="260"/>
-      <c r="I22" s="260"/>
+      <c r="H22" s="252"/>
+      <c r="I22" s="252"/>
       <c r="J22" s="103"/>
     </row>
     <row r="23" spans="1:10" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="92"/>
-      <c r="B23" s="259" t="s">
+      <c r="B23" s="251" t="s">
         <v>141</v>
       </c>
-      <c r="C23" s="259"/>
-      <c r="D23" s="259"/>
-      <c r="E23" s="259"/>
-      <c r="F23" s="259"/>
+      <c r="C23" s="251"/>
+      <c r="D23" s="251"/>
+      <c r="E23" s="251"/>
+      <c r="F23" s="251"/>
       <c r="G23" s="105">
         <v>100</v>
       </c>
-      <c r="H23" s="260"/>
-      <c r="I23" s="260"/>
+      <c r="H23" s="252"/>
+      <c r="I23" s="252"/>
       <c r="J23" s="103"/>
     </row>
     <row r="24" spans="1:10" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="92"/>
-      <c r="B24" s="259" t="s">
+      <c r="B24" s="251" t="s">
         <v>142</v>
       </c>
-      <c r="C24" s="259"/>
-      <c r="D24" s="259"/>
-      <c r="E24" s="259"/>
-      <c r="F24" s="259"/>
+      <c r="C24" s="251"/>
+      <c r="D24" s="251"/>
+      <c r="E24" s="251"/>
+      <c r="F24" s="251"/>
       <c r="G24" s="105">
         <v>1840</v>
       </c>
-      <c r="H24" s="260"/>
-      <c r="I24" s="260"/>
+      <c r="H24" s="252"/>
+      <c r="I24" s="252"/>
       <c r="J24" s="103"/>
     </row>
     <row r="25" spans="1:10" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="92"/>
-      <c r="B25" s="259" t="s">
+      <c r="B25" s="251" t="s">
         <v>143</v>
       </c>
-      <c r="C25" s="259"/>
-      <c r="D25" s="259"/>
-      <c r="E25" s="259"/>
-      <c r="F25" s="259"/>
+      <c r="C25" s="251"/>
+      <c r="D25" s="251"/>
+      <c r="E25" s="251"/>
+      <c r="F25" s="251"/>
       <c r="G25" s="105">
         <v>202</v>
       </c>
-      <c r="H25" s="260"/>
-      <c r="I25" s="260"/>
+      <c r="H25" s="252"/>
+      <c r="I25" s="252"/>
       <c r="J25" s="103"/>
     </row>
     <row r="26" spans="1:10" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="92"/>
-      <c r="B26" s="259" t="s">
+      <c r="B26" s="251" t="s">
         <v>144</v>
       </c>
-      <c r="C26" s="259"/>
-      <c r="D26" s="259"/>
-      <c r="E26" s="259"/>
-      <c r="F26" s="259"/>
+      <c r="C26" s="251"/>
+      <c r="D26" s="251"/>
+      <c r="E26" s="251"/>
+      <c r="F26" s="251"/>
       <c r="G26" s="105"/>
-      <c r="H26" s="260"/>
-      <c r="I26" s="260"/>
+      <c r="H26" s="252"/>
+      <c r="I26" s="252"/>
       <c r="J26" s="103"/>
     </row>
     <row r="27" spans="1:10" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="92"/>
-      <c r="B27" s="259" t="s">
+      <c r="B27" s="251" t="s">
         <v>145</v>
       </c>
-      <c r="C27" s="259"/>
-      <c r="D27" s="259"/>
-      <c r="E27" s="259"/>
-      <c r="F27" s="259"/>
+      <c r="C27" s="251"/>
+      <c r="D27" s="251"/>
+      <c r="E27" s="251"/>
+      <c r="F27" s="251"/>
       <c r="G27" s="104">
         <f>SUM(G22:G26)</f>
         <v>3142</v>
       </c>
-      <c r="H27" s="261">
+      <c r="H27" s="253">
         <f>SUM(I22:I26)</f>
         <v>0</v>
       </c>
-      <c r="I27" s="261"/>
+      <c r="I27" s="253"/>
       <c r="J27" s="110">
         <f>G27+H27</f>
         <v>3142</v>
@@ -27284,24 +27295,6 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="31">
-    <mergeCell ref="B25:F25"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="B26:F26"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="B27:F27"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="B22:F22"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="B23:F23"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="B24:F24"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="B18:F18"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="B19:F19"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="B21:F21"/>
-    <mergeCell ref="H21:I21"/>
     <mergeCell ref="B17:F17"/>
     <mergeCell ref="H17:I17"/>
     <mergeCell ref="A1:J1"/>
@@ -27315,6 +27308,24 @@
     <mergeCell ref="H15:I15"/>
     <mergeCell ref="B16:F16"/>
     <mergeCell ref="H16:I16"/>
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="B19:F19"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="B25:F25"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="B26:F26"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="B27:F27"/>
+    <mergeCell ref="H27:I27"/>
   </mergeCells>
   <pageMargins left="0.55972222222222223" right="0.50972222222222219" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555551" footer="0.51180555555555551"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -27344,18 +27355,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="262" t="s">
+      <c r="A1" s="267" t="s">
         <v>153</v>
       </c>
-      <c r="B1" s="262"/>
-      <c r="C1" s="262"/>
-      <c r="D1" s="262"/>
-      <c r="E1" s="262"/>
-      <c r="F1" s="262"/>
-      <c r="G1" s="262"/>
-      <c r="H1" s="262"/>
-      <c r="I1" s="262"/>
-      <c r="J1" s="262"/>
+      <c r="B1" s="267"/>
+      <c r="C1" s="267"/>
+      <c r="D1" s="267"/>
+      <c r="E1" s="267"/>
+      <c r="F1" s="267"/>
+      <c r="G1" s="267"/>
+      <c r="H1" s="267"/>
+      <c r="I1" s="267"/>
+      <c r="J1" s="267"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="118"/>
@@ -27459,57 +27470,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="264" t="s">
+      <c r="A1" s="272" t="s">
         <v>162</v>
       </c>
-      <c r="B1" s="264"/>
-      <c r="C1" s="264"/>
-      <c r="D1" s="264"/>
-      <c r="E1" s="264"/>
+      <c r="B1" s="272"/>
+      <c r="C1" s="272"/>
+      <c r="D1" s="272"/>
+      <c r="E1" s="272"/>
     </row>
     <row r="2" spans="1:5" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="123" t="s">
         <v>163</v>
       </c>
-      <c r="B2" s="265">
+      <c r="B2" s="273">
         <f>IF(ISBLANK(Seznam_do_35_účastníků!C6)," ",Seznam_do_35_účastníků!C6)</f>
         <v>0</v>
       </c>
-      <c r="C2" s="265"/>
-      <c r="D2" s="265"/>
-      <c r="E2" s="265"/>
+      <c r="C2" s="273"/>
+      <c r="D2" s="273"/>
+      <c r="E2" s="273"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="124" t="s">
         <v>164</v>
       </c>
-      <c r="B3" s="265" t="str">
+      <c r="B3" s="273" t="str">
         <f>IF(ISBLANK(Seznam_do_35_účastníků!C2)," ",Seznam_do_35_účastníků!C2)</f>
         <v>Šán</v>
       </c>
-      <c r="C3" s="265"/>
-      <c r="D3" s="265"/>
-      <c r="E3" s="265"/>
+      <c r="C3" s="273"/>
+      <c r="D3" s="273"/>
+      <c r="E3" s="273"/>
     </row>
     <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="124" t="s">
         <v>165</v>
       </c>
-      <c r="B4" s="266" t="str">
+      <c r="B4" s="274" t="str">
         <f ca="1">IF(AND(ISNUMBER('Seznam účastníků'!B5),ISNUMBER('Seznam účastníků'!B6)),IF(ISNUMBER(VALUE(TEXT(TODAY(),"rrrr"))),TEXT('Seznam účastníků'!B5,"dd.mm.rrrr")&amp;" - "&amp;TEXT('Seznam účastníků'!B6,"dd.mm.rrrr"),TEXT('Seznam účastníků'!B5,"dd.mm.yyyy")&amp;" - "&amp;TEXT('Seznam účastníků'!B6,"dd.mm.yyyy"))," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="C4" s="266"/>
-      <c r="D4" s="266"/>
-      <c r="E4" s="266"/>
+      <c r="C4" s="274"/>
+      <c r="D4" s="274"/>
+      <c r="E4" s="274"/>
     </row>
     <row r="5" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A5" s="125"/>
-      <c r="B5" s="267" t="s">
+      <c r="B5" s="275" t="s">
         <v>166</v>
       </c>
-      <c r="C5" s="267"/>
-      <c r="D5" s="267"/>
+      <c r="C5" s="275"/>
+      <c r="D5" s="275"/>
       <c r="E5" s="126" t="s">
         <v>167</v>
       </c>
@@ -27761,13 +27772,13 @@
       <c r="E21" s="90"/>
     </row>
     <row r="22" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="263" t="s">
+      <c r="A22" s="271" t="s">
         <v>178</v>
       </c>
-      <c r="B22" s="263"/>
-      <c r="C22" s="263"/>
-      <c r="D22" s="263"/>
-      <c r="E22" s="263"/>
+      <c r="B22" s="271"/>
+      <c r="C22" s="271"/>
+      <c r="D22" s="271"/>
+      <c r="E22" s="271"/>
     </row>
     <row r="23" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="146" t="s">
@@ -27915,6 +27926,12 @@
   </sheetData>
   <sheetProtection sheet="1"/>
   <mergeCells count="16">
+    <mergeCell ref="A22:E22"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:D5"/>
     <mergeCell ref="C29:E29"/>
     <mergeCell ref="C30:E30"/>
     <mergeCell ref="C31:E31"/>
@@ -27925,12 +27942,6 @@
     <mergeCell ref="C26:E26"/>
     <mergeCell ref="C27:E27"/>
     <mergeCell ref="C28:E28"/>
-    <mergeCell ref="A22:E22"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:D5"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555551" footer="0.51180555555555551"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -27940,7 +27951,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:L99"/>
+  <dimension ref="A1:L109"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -27948,7 +27959,7 @@
   <cols>
     <col min="1" max="1" width="17.42578125" style="156" customWidth="1"/>
     <col min="2" max="2" width="12.7109375" style="156" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" style="284" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" style="220" customWidth="1"/>
     <col min="4" max="4" width="20.140625" style="156" customWidth="1"/>
     <col min="5" max="5" width="10.140625" style="156" customWidth="1"/>
     <col min="6" max="6" width="9" style="156"/>
@@ -27980,8 +27991,8 @@
       <c r="A4" s="156" t="s">
         <v>193</v>
       </c>
-      <c r="B4" s="271"/>
-      <c r="C4" s="271"/>
+      <c r="B4" s="276"/>
+      <c r="C4" s="276"/>
       <c r="D4"/>
       <c r="G4" s="159"/>
     </row>
@@ -27989,8 +28000,8 @@
       <c r="A5" s="156" t="s">
         <v>194</v>
       </c>
-      <c r="B5" s="285"/>
-      <c r="C5" s="285"/>
+      <c r="B5" s="277"/>
+      <c r="C5" s="277"/>
       <c r="D5"/>
       <c r="G5" s="159"/>
     </row>
@@ -27998,8 +28009,8 @@
       <c r="A6" s="156" t="s">
         <v>195</v>
       </c>
-      <c r="B6" s="285"/>
-      <c r="C6" s="285"/>
+      <c r="B6" s="277"/>
+      <c r="C6" s="277"/>
       <c r="D6"/>
       <c r="G6" s="159"/>
     </row>
@@ -28007,8 +28018,8 @@
       <c r="A7" s="156" t="s">
         <v>196</v>
       </c>
-      <c r="B7" s="271"/>
-      <c r="C7" s="271"/>
+      <c r="B7" s="276"/>
+      <c r="C7" s="276"/>
       <c r="D7"/>
       <c r="G7" s="159"/>
     </row>
@@ -28089,10 +28100,10 @@
       <c r="G15" s="159"/>
     </row>
     <row r="16" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A16" s="272" t="s">
+      <c r="A16" s="278" t="s">
         <v>203</v>
       </c>
-      <c r="B16" s="272"/>
+      <c r="B16" s="278"/>
       <c r="C16" s="156"/>
       <c r="G16" s="159"/>
     </row>
@@ -28127,7 +28138,7 @@
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="171"/>
       <c r="B19" s="172"/>
-      <c r="C19" s="280"/>
+      <c r="C19" s="216"/>
       <c r="D19" s="172"/>
       <c r="E19" s="172"/>
       <c r="F19" s="173"/>
@@ -28137,7 +28148,7 @@
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="171"/>
       <c r="B20" s="176"/>
-      <c r="C20" s="280"/>
+      <c r="C20" s="216"/>
       <c r="D20" s="176"/>
       <c r="E20" s="172"/>
       <c r="F20" s="173"/>
@@ -28150,7 +28161,7 @@
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" s="171"/>
       <c r="B21" s="172"/>
-      <c r="C21" s="280"/>
+      <c r="C21" s="216"/>
       <c r="D21" s="172"/>
       <c r="E21" s="172"/>
       <c r="F21" s="173"/>
@@ -28159,7 +28170,7 @@
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="171"/>
       <c r="B22" s="176"/>
-      <c r="C22" s="280"/>
+      <c r="C22" s="216"/>
       <c r="D22" s="176"/>
       <c r="E22" s="172"/>
       <c r="F22" s="173"/>
@@ -28172,7 +28183,7 @@
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="171"/>
       <c r="B23" s="178"/>
-      <c r="C23" s="280"/>
+      <c r="C23" s="216"/>
       <c r="D23" s="178"/>
       <c r="E23" s="172"/>
       <c r="F23" s="173"/>
@@ -28181,7 +28192,7 @@
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="171"/>
       <c r="B24" s="172"/>
-      <c r="C24" s="280"/>
+      <c r="C24" s="216"/>
       <c r="D24" s="172"/>
       <c r="E24" s="172"/>
       <c r="F24" s="173"/>
@@ -28191,7 +28202,7 @@
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" s="171"/>
       <c r="B25" s="179"/>
-      <c r="C25" s="280"/>
+      <c r="C25" s="216"/>
       <c r="D25" s="179"/>
       <c r="E25" s="172"/>
       <c r="F25" s="173"/>
@@ -28200,7 +28211,7 @@
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" s="171"/>
       <c r="B26" s="176"/>
-      <c r="C26" s="280"/>
+      <c r="C26" s="216"/>
       <c r="D26" s="176"/>
       <c r="E26" s="172"/>
       <c r="F26" s="173"/>
@@ -28210,7 +28221,7 @@
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" s="171"/>
       <c r="B27" s="172"/>
-      <c r="C27" s="280"/>
+      <c r="C27" s="216"/>
       <c r="D27" s="172"/>
       <c r="E27" s="172"/>
       <c r="F27" s="173"/>
@@ -28220,7 +28231,7 @@
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" s="171"/>
       <c r="B28" s="178"/>
-      <c r="C28" s="280"/>
+      <c r="C28" s="216"/>
       <c r="D28" s="178"/>
       <c r="E28" s="172"/>
       <c r="F28" s="173"/>
@@ -28231,7 +28242,7 @@
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" s="171"/>
       <c r="B29" s="178"/>
-      <c r="C29" s="280"/>
+      <c r="C29" s="216"/>
       <c r="D29" s="178"/>
       <c r="E29" s="172"/>
       <c r="F29" s="173"/>
@@ -28242,7 +28253,7 @@
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" s="171"/>
       <c r="B30" s="178"/>
-      <c r="C30" s="280"/>
+      <c r="C30" s="216"/>
       <c r="D30" s="178"/>
       <c r="E30" s="172"/>
       <c r="F30" s="173"/>
@@ -28253,7 +28264,7 @@
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" s="180"/>
       <c r="B31" s="178"/>
-      <c r="C31" s="280"/>
+      <c r="C31" s="216"/>
       <c r="D31" s="178"/>
       <c r="E31" s="172"/>
       <c r="F31" s="173"/>
@@ -28264,7 +28275,7 @@
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" s="157"/>
       <c r="B32" s="178"/>
-      <c r="C32" s="280"/>
+      <c r="C32" s="216"/>
       <c r="D32" s="171"/>
       <c r="E32" s="172"/>
       <c r="F32" s="173"/>
@@ -28275,7 +28286,7 @@
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="157"/>
       <c r="B33" s="178"/>
-      <c r="C33" s="281"/>
+      <c r="C33" s="217"/>
       <c r="D33" s="178"/>
       <c r="E33" s="172"/>
       <c r="F33" s="173"/>
@@ -28286,7 +28297,7 @@
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="157"/>
       <c r="B34" s="178"/>
-      <c r="C34" s="282"/>
+      <c r="C34" s="218"/>
       <c r="D34" s="171"/>
       <c r="E34" s="171"/>
       <c r="F34" s="173"/>
@@ -28297,7 +28308,7 @@
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="157"/>
       <c r="B35" s="157"/>
-      <c r="C35" s="283"/>
+      <c r="C35" s="219"/>
       <c r="D35" s="171"/>
       <c r="E35" s="171"/>
       <c r="F35" s="173"/>
@@ -28306,7 +28317,7 @@
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="157"/>
       <c r="B36" s="157"/>
-      <c r="C36" s="283"/>
+      <c r="C36" s="219"/>
       <c r="D36" s="171"/>
       <c r="E36" s="171"/>
       <c r="F36" s="173"/>
@@ -28315,7 +28326,7 @@
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="157"/>
       <c r="B37" s="157"/>
-      <c r="C37" s="283"/>
+      <c r="C37" s="219"/>
       <c r="D37" s="157"/>
       <c r="E37" s="181"/>
       <c r="F37" s="173"/>
@@ -28324,7 +28335,7 @@
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="157"/>
       <c r="B38" s="157"/>
-      <c r="C38" s="283"/>
+      <c r="C38" s="219"/>
       <c r="D38" s="157"/>
       <c r="E38" s="181"/>
       <c r="F38" s="173"/>
@@ -28333,7 +28344,7 @@
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" s="157"/>
       <c r="B39" s="157"/>
-      <c r="C39" s="283"/>
+      <c r="C39" s="219"/>
       <c r="D39" s="157"/>
       <c r="E39" s="181"/>
       <c r="F39" s="173"/>
@@ -28342,7 +28353,7 @@
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" s="157"/>
       <c r="B40" s="157"/>
-      <c r="C40" s="283"/>
+      <c r="C40" s="219"/>
       <c r="D40" s="157"/>
       <c r="E40" s="181"/>
       <c r="F40" s="173"/>
@@ -28351,7 +28362,7 @@
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" s="157"/>
       <c r="B41" s="157"/>
-      <c r="C41" s="283"/>
+      <c r="C41" s="219"/>
       <c r="D41" s="157"/>
       <c r="E41" s="181"/>
       <c r="F41" s="173"/>
@@ -28360,7 +28371,7 @@
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="157"/>
       <c r="B42" s="157"/>
-      <c r="C42" s="283"/>
+      <c r="C42" s="219"/>
       <c r="D42" s="157"/>
       <c r="E42" s="181"/>
       <c r="F42" s="173"/>
@@ -28369,7 +28380,7 @@
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" s="157"/>
       <c r="B43" s="157"/>
-      <c r="C43" s="283"/>
+      <c r="C43" s="219"/>
       <c r="D43" s="157"/>
       <c r="E43" s="181"/>
       <c r="F43" s="173"/>
@@ -28378,7 +28389,7 @@
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="157"/>
       <c r="B44" s="157"/>
-      <c r="C44" s="283"/>
+      <c r="C44" s="219"/>
       <c r="D44" s="157"/>
       <c r="E44" s="157"/>
       <c r="F44" s="173"/>
@@ -28387,7 +28398,7 @@
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" s="157"/>
       <c r="B45" s="157"/>
-      <c r="C45" s="283"/>
+      <c r="C45" s="219"/>
       <c r="D45" s="157"/>
       <c r="E45" s="157"/>
       <c r="F45" s="173"/>
@@ -28396,7 +28407,7 @@
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" s="157"/>
       <c r="B46" s="157"/>
-      <c r="C46" s="283"/>
+      <c r="C46" s="219"/>
       <c r="D46" s="157"/>
       <c r="E46" s="157"/>
       <c r="F46" s="173"/>
@@ -28405,7 +28416,7 @@
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="157"/>
       <c r="B47" s="157"/>
-      <c r="C47" s="283"/>
+      <c r="C47" s="219"/>
       <c r="D47" s="157"/>
       <c r="E47" s="157"/>
       <c r="F47" s="173"/>
@@ -28414,418 +28425,500 @@
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" s="157"/>
       <c r="B48" s="157"/>
-      <c r="C48" s="283"/>
+      <c r="C48" s="219"/>
       <c r="D48" s="157"/>
       <c r="E48" s="157"/>
       <c r="F48" s="173"/>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G48" s="286"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" s="157"/>
       <c r="B49" s="157"/>
-      <c r="C49" s="283"/>
+      <c r="C49" s="219"/>
       <c r="D49" s="157"/>
       <c r="E49" s="157"/>
       <c r="F49" s="173"/>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G49" s="286"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" s="157"/>
       <c r="B50" s="157"/>
-      <c r="C50" s="283"/>
+      <c r="C50" s="219"/>
       <c r="D50" s="157"/>
       <c r="E50" s="157"/>
       <c r="F50" s="173"/>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G50" s="286"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" s="157"/>
       <c r="B51" s="157"/>
-      <c r="C51" s="283"/>
+      <c r="C51" s="219"/>
       <c r="D51" s="157"/>
       <c r="E51" s="157"/>
       <c r="F51" s="173"/>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G51" s="286"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" s="157"/>
       <c r="B52" s="157"/>
-      <c r="C52" s="283"/>
+      <c r="C52" s="219"/>
       <c r="D52" s="157"/>
       <c r="E52" s="157"/>
       <c r="F52" s="173"/>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G52" s="286"/>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" s="157"/>
       <c r="B53" s="157"/>
-      <c r="C53" s="283"/>
+      <c r="C53" s="219"/>
       <c r="D53" s="157"/>
       <c r="E53" s="157"/>
       <c r="F53" s="173"/>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G53" s="286"/>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" s="157"/>
       <c r="B54" s="157"/>
-      <c r="C54" s="283"/>
+      <c r="C54" s="219"/>
       <c r="D54" s="157"/>
       <c r="E54" s="157"/>
       <c r="F54" s="173"/>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G54" s="286"/>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" s="157"/>
       <c r="B55" s="157"/>
-      <c r="C55" s="283"/>
+      <c r="C55" s="219"/>
       <c r="D55" s="157"/>
       <c r="E55" s="157"/>
       <c r="F55" s="173"/>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G55" s="286"/>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" s="157"/>
       <c r="B56" s="157"/>
-      <c r="C56" s="283"/>
+      <c r="C56" s="219"/>
       <c r="D56" s="157"/>
       <c r="E56" s="157"/>
       <c r="F56" s="173"/>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G56" s="286"/>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" s="157"/>
       <c r="B57" s="157"/>
-      <c r="C57" s="283"/>
+      <c r="C57" s="219"/>
       <c r="D57" s="157"/>
       <c r="E57" s="157"/>
       <c r="F57" s="173"/>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G57" s="286"/>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" s="157"/>
       <c r="B58" s="157"/>
-      <c r="C58" s="283"/>
+      <c r="C58" s="219"/>
       <c r="D58" s="157"/>
       <c r="E58" s="157"/>
       <c r="F58" s="173"/>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G58" s="286"/>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" s="157"/>
       <c r="B59" s="157"/>
-      <c r="C59" s="283"/>
+      <c r="C59" s="219"/>
       <c r="D59" s="157"/>
       <c r="E59" s="157"/>
       <c r="F59" s="173"/>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G59" s="286"/>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" s="157"/>
       <c r="B60" s="157"/>
-      <c r="C60" s="283"/>
+      <c r="C60" s="219"/>
       <c r="D60" s="157"/>
       <c r="E60" s="157"/>
       <c r="F60" s="173"/>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G60" s="286"/>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" s="157"/>
       <c r="B61" s="157"/>
-      <c r="C61" s="283"/>
+      <c r="C61" s="219"/>
       <c r="D61" s="157"/>
       <c r="E61" s="157"/>
       <c r="F61" s="173"/>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G61" s="286"/>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" s="157"/>
       <c r="B62" s="157"/>
-      <c r="C62" s="283"/>
+      <c r="C62" s="219"/>
       <c r="D62" s="157"/>
       <c r="E62" s="157"/>
       <c r="F62" s="173"/>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G62" s="286"/>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" s="157"/>
       <c r="B63" s="157"/>
-      <c r="C63" s="283"/>
+      <c r="C63" s="219"/>
       <c r="D63" s="157"/>
       <c r="E63" s="157"/>
       <c r="F63" s="173"/>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G63" s="286"/>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" s="157"/>
       <c r="B64" s="157"/>
-      <c r="C64" s="283"/>
+      <c r="C64" s="219"/>
       <c r="D64" s="157"/>
       <c r="E64" s="157"/>
       <c r="F64" s="173"/>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G64" s="286"/>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" s="157"/>
       <c r="B65" s="157"/>
-      <c r="C65" s="283"/>
+      <c r="C65" s="219"/>
       <c r="D65" s="157"/>
       <c r="E65" s="157"/>
       <c r="F65" s="173"/>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G65" s="286"/>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" s="157"/>
       <c r="B66" s="157"/>
-      <c r="C66" s="283"/>
+      <c r="C66" s="219"/>
       <c r="D66" s="157"/>
       <c r="E66" s="157"/>
       <c r="F66" s="173"/>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G66" s="286"/>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" s="157"/>
       <c r="B67" s="157"/>
-      <c r="C67" s="283"/>
+      <c r="C67" s="219"/>
       <c r="D67" s="157"/>
       <c r="E67" s="157"/>
       <c r="F67" s="173"/>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G67" s="286"/>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" s="157"/>
       <c r="B68" s="157"/>
-      <c r="C68" s="283"/>
+      <c r="C68" s="219"/>
       <c r="D68" s="157"/>
       <c r="E68" s="157"/>
       <c r="F68" s="173"/>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G68" s="286"/>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" s="157"/>
       <c r="B69" s="157"/>
-      <c r="C69" s="283"/>
+      <c r="C69" s="219"/>
       <c r="D69" s="157"/>
       <c r="E69" s="157"/>
       <c r="F69" s="173"/>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G69" s="286"/>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" s="157"/>
       <c r="B70" s="157"/>
-      <c r="C70" s="283"/>
+      <c r="C70" s="219"/>
       <c r="D70" s="157"/>
       <c r="E70" s="157"/>
       <c r="F70" s="157"/>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G70" s="286"/>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" s="157"/>
       <c r="B71" s="157"/>
-      <c r="C71" s="283"/>
+      <c r="C71" s="219"/>
       <c r="D71" s="157"/>
       <c r="E71" s="157"/>
       <c r="F71" s="157"/>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G71" s="286"/>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72" s="157"/>
       <c r="B72" s="157"/>
-      <c r="C72" s="283"/>
+      <c r="C72" s="219"/>
       <c r="D72" s="157"/>
       <c r="E72" s="157"/>
       <c r="F72" s="157"/>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G72" s="286"/>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73" s="157"/>
       <c r="B73" s="157"/>
-      <c r="C73" s="283"/>
+      <c r="C73" s="219"/>
       <c r="D73" s="157"/>
       <c r="E73" s="157"/>
       <c r="F73" s="157"/>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G73" s="286"/>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74" s="157"/>
       <c r="B74" s="157"/>
-      <c r="C74" s="283"/>
+      <c r="C74" s="219"/>
       <c r="D74" s="157"/>
       <c r="E74" s="157"/>
       <c r="F74" s="157"/>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G74" s="286"/>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75" s="157"/>
       <c r="B75" s="157"/>
-      <c r="C75" s="283"/>
+      <c r="C75" s="219"/>
       <c r="D75" s="157"/>
       <c r="E75" s="157"/>
       <c r="F75" s="157"/>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G75" s="286"/>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" s="157"/>
       <c r="B76" s="157"/>
-      <c r="C76" s="283"/>
+      <c r="C76" s="219"/>
       <c r="D76" s="157"/>
       <c r="E76" s="157"/>
       <c r="F76" s="157"/>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G76" s="286"/>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77" s="157"/>
       <c r="B77" s="157"/>
-      <c r="C77" s="283"/>
+      <c r="C77" s="219"/>
       <c r="D77" s="157"/>
       <c r="E77" s="157"/>
       <c r="F77" s="157"/>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G77" s="286"/>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78" s="157"/>
       <c r="B78" s="157"/>
-      <c r="C78" s="283"/>
+      <c r="C78" s="219"/>
       <c r="D78" s="157"/>
       <c r="E78" s="157"/>
       <c r="F78" s="157"/>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G78" s="286"/>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79" s="157"/>
       <c r="B79" s="157"/>
-      <c r="C79" s="283"/>
+      <c r="C79" s="219"/>
       <c r="D79" s="157"/>
       <c r="E79" s="157"/>
       <c r="F79" s="157"/>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G79" s="286"/>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80" s="157"/>
       <c r="B80" s="157"/>
-      <c r="C80" s="283"/>
+      <c r="C80" s="219"/>
       <c r="D80" s="157"/>
       <c r="E80" s="157"/>
       <c r="F80" s="157"/>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G80" s="286"/>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81" s="157"/>
       <c r="B81" s="157"/>
-      <c r="C81" s="283"/>
+      <c r="C81" s="219"/>
       <c r="D81" s="157"/>
       <c r="E81" s="157"/>
       <c r="F81" s="157"/>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G81" s="286"/>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" s="157"/>
       <c r="B82" s="157"/>
-      <c r="C82" s="283"/>
+      <c r="C82" s="219"/>
       <c r="D82" s="157"/>
       <c r="E82" s="157"/>
       <c r="F82" s="157"/>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G82" s="286"/>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83" s="157"/>
       <c r="B83" s="157"/>
-      <c r="C83" s="283"/>
+      <c r="C83" s="219"/>
       <c r="D83" s="157"/>
       <c r="E83" s="157"/>
       <c r="F83" s="157"/>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G83" s="286"/>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84" s="157"/>
       <c r="B84" s="157"/>
-      <c r="C84" s="283"/>
+      <c r="C84" s="219"/>
       <c r="D84" s="157"/>
       <c r="E84" s="157"/>
       <c r="F84" s="157"/>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G84" s="286"/>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85" s="157"/>
       <c r="B85" s="157"/>
-      <c r="C85" s="283"/>
+      <c r="C85" s="219"/>
       <c r="D85" s="157"/>
       <c r="E85" s="157"/>
       <c r="F85" s="157"/>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G85" s="286"/>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86" s="157"/>
       <c r="B86" s="157"/>
-      <c r="C86" s="283"/>
+      <c r="C86" s="219"/>
       <c r="D86" s="157"/>
       <c r="E86" s="157"/>
       <c r="F86" s="157"/>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G86" s="286"/>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87" s="157"/>
       <c r="B87" s="157"/>
-      <c r="C87" s="283"/>
+      <c r="C87" s="219"/>
       <c r="D87" s="157"/>
       <c r="E87" s="157"/>
       <c r="F87" s="157"/>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G87" s="286"/>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88" s="157"/>
       <c r="B88" s="157"/>
-      <c r="C88" s="283"/>
+      <c r="C88" s="219"/>
       <c r="D88" s="157"/>
       <c r="E88" s="157"/>
       <c r="F88" s="157"/>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G88" s="286"/>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A89" s="157"/>
       <c r="B89" s="157"/>
-      <c r="C89" s="283"/>
+      <c r="C89" s="219"/>
       <c r="D89" s="157"/>
       <c r="E89" s="157"/>
       <c r="F89" s="157"/>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G89" s="286"/>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90" s="157"/>
       <c r="B90" s="157"/>
-      <c r="C90" s="283"/>
+      <c r="C90" s="219"/>
       <c r="D90" s="157"/>
       <c r="E90" s="157"/>
       <c r="F90" s="157"/>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G90" s="286"/>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A91" s="157"/>
       <c r="B91" s="157"/>
-      <c r="C91" s="283"/>
+      <c r="C91" s="219"/>
       <c r="D91" s="157"/>
       <c r="E91" s="157"/>
       <c r="F91" s="157"/>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G91" s="286"/>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A92" s="157"/>
       <c r="B92" s="157"/>
-      <c r="C92" s="283"/>
+      <c r="C92" s="219"/>
       <c r="D92" s="157"/>
       <c r="E92" s="157"/>
       <c r="F92" s="157"/>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G92" s="286"/>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A93" s="157"/>
       <c r="B93" s="157"/>
-      <c r="C93" s="283"/>
+      <c r="C93" s="219"/>
       <c r="D93" s="157"/>
       <c r="E93" s="157"/>
       <c r="F93" s="157"/>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G93" s="286"/>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A94" s="157"/>
       <c r="B94" s="157"/>
-      <c r="C94" s="283"/>
+      <c r="C94" s="219"/>
       <c r="D94" s="157"/>
       <c r="E94" s="157"/>
       <c r="F94" s="157"/>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G94" s="286"/>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A95" s="157"/>
       <c r="B95" s="157"/>
-      <c r="C95" s="283"/>
+      <c r="C95" s="219"/>
       <c r="D95" s="157"/>
       <c r="E95" s="157"/>
       <c r="F95" s="157"/>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G95" s="286"/>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A96" s="157"/>
       <c r="B96" s="157"/>
-      <c r="C96" s="283"/>
+      <c r="C96" s="219"/>
       <c r="D96" s="157"/>
       <c r="E96" s="157"/>
       <c r="F96" s="157"/>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G96" s="286"/>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A97" s="157"/>
       <c r="B97" s="157"/>
-      <c r="C97" s="283"/>
+      <c r="C97" s="219"/>
       <c r="D97" s="157"/>
       <c r="E97" s="157"/>
       <c r="F97" s="157"/>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G97" s="286"/>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A98" s="157"/>
       <c r="B98" s="157"/>
-      <c r="C98" s="283"/>
+      <c r="C98" s="219"/>
       <c r="D98" s="157"/>
       <c r="E98" s="157"/>
       <c r="F98" s="157"/>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G98" s="286"/>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A99" s="157"/>
       <c r="B99" s="157"/>
-      <c r="C99" s="283"/>
+      <c r="C99" s="219"/>
       <c r="D99" s="157"/>
       <c r="E99" s="157"/>
       <c r="F99" s="157"/>
+      <c r="G99" s="286"/>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G100" s="286"/>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G101" s="286"/>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G102" s="286"/>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G103" s="286"/>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G104" s="286"/>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G105" s="286"/>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G106" s="286"/>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G107" s="286"/>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G108" s="286"/>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G109" s="286"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1"/>
@@ -28876,11 +28969,11 @@
       <c r="A4" s="156" t="s">
         <v>193</v>
       </c>
-      <c r="B4" s="273">
+      <c r="B4" s="279">
         <f>'Seznam účastníků'!B4</f>
         <v>0</v>
       </c>
-      <c r="C4" s="273"/>
+      <c r="C4" s="279"/>
       <c r="D4"/>
       <c r="E4"/>
     </row>
@@ -28888,11 +28981,11 @@
       <c r="A5" s="156" t="s">
         <v>194</v>
       </c>
-      <c r="B5" s="274">
+      <c r="B5" s="280">
         <f>'Seznam účastníků'!B5</f>
         <v>0</v>
       </c>
-      <c r="C5" s="274"/>
+      <c r="C5" s="280"/>
       <c r="D5"/>
       <c r="E5"/>
     </row>
@@ -28900,11 +28993,11 @@
       <c r="A6" s="156" t="s">
         <v>195</v>
       </c>
-      <c r="B6" s="274">
+      <c r="B6" s="280">
         <f>'Seznam účastníků'!B6</f>
         <v>0</v>
       </c>
-      <c r="C6" s="274"/>
+      <c r="C6" s="280"/>
       <c r="D6"/>
       <c r="E6"/>
     </row>
@@ -28912,11 +29005,11 @@
       <c r="A7" s="156" t="s">
         <v>196</v>
       </c>
-      <c r="B7" s="273">
+      <c r="B7" s="279">
         <f>'Seznam účastníků'!B7</f>
         <v>0</v>
       </c>
-      <c r="C7" s="273"/>
+      <c r="C7" s="279"/>
       <c r="D7"/>
       <c r="E7"/>
     </row>

</xml_diff>